<commit_message>
JM and JA updates to data_combination and JP added TAC
</commit_message>
<xml_diff>
--- a/data/agage/data_combination.xlsx
+++ b/data/agage/data_combination.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/code/agage-archive/data/data_selection/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0288E0D-E5AF-4E49-A82D-95B3D8E9601E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD583BD7-92F8-CB41-86FB-6519BF7E8268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="1100" windowWidth="27240" windowHeight="16440" activeTab="8" xr2:uid="{9985A75E-EB26-5749-BA8E-B1A91FE63120}"/>
+    <workbookView xWindow="9500" yWindow="500" windowWidth="26000" windowHeight="21100" activeTab="9" xr2:uid="{9985A75E-EB26-5749-BA8E-B1A91FE63120}"/>
   </bookViews>
   <sheets>
     <sheet name="CGO" sheetId="1" r:id="rId1"/>
-    <sheet name="CMO" sheetId="9" r:id="rId2"/>
-    <sheet name="MHD" sheetId="2" r:id="rId3"/>
-    <sheet name="THD" sheetId="3" r:id="rId4"/>
-    <sheet name="RPB" sheetId="4" r:id="rId5"/>
-    <sheet name="SMO" sheetId="5" r:id="rId6"/>
-    <sheet name="ZEP" sheetId="6" r:id="rId7"/>
-    <sheet name="JFJ" sheetId="10" r:id="rId8"/>
-    <sheet name="CMN" sheetId="7" r:id="rId9"/>
+    <sheet name="CMN" sheetId="7" r:id="rId2"/>
+    <sheet name="CMO" sheetId="9" r:id="rId3"/>
+    <sheet name="JFJ" sheetId="10" r:id="rId4"/>
+    <sheet name="MHD" sheetId="2" r:id="rId5"/>
+    <sheet name="RPB" sheetId="4" r:id="rId6"/>
+    <sheet name="SMO" sheetId="5" r:id="rId7"/>
+    <sheet name="TAC" sheetId="13" r:id="rId8"/>
+    <sheet name="THD" sheetId="3" r:id="rId9"/>
+    <sheet name="ZEP" sheetId="6" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -47,7 +48,11 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={E2A43AB0-C9B5-4349-922D-876081C672EC}</author>
+    <author>tc={E55AD725-15DB-43AB-8E3D-FF58A480B65B}</author>
+    <author>tc={5540EEFA-5767-4C3A-97E4-DDFAA77A7BDD}</author>
     <author>tc={E74B7E44-2395-6C42-B73D-2EC1F22A60C7}</author>
+    <author>tc={E9B3D22A-D92F-42DF-B73C-1C78227D06FF}</author>
+    <author>tc={A83E3842-9BE6-4EA3-92B3-E3B0D5967A00}</author>
   </authors>
   <commentList>
     <comment ref="E9" authorId="0" shapeId="0" xr:uid="{E2A43AB0-C9B5-4349-922D-876081C672EC}">
@@ -58,12 +63,44 @@
     I just made these CH4 dates up for testing</t>
       </text>
     </comment>
-    <comment ref="C11" authorId="1" shapeId="0" xr:uid="{E74B7E44-2395-6C42-B73D-2EC1F22A60C7}">
+    <comment ref="G10" authorId="1" shapeId="0" xr:uid="{E55AD725-15DB-43AB-8E3D-FF58A480B65B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    PBK cut off dates</t>
+      </text>
+    </comment>
+    <comment ref="J10" authorId="2" shapeId="0" xr:uid="{5540EEFA-5767-4C3A-97E4-DDFAA77A7BDD}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    PBK cut off dates</t>
+      </text>
+    </comment>
+    <comment ref="C11" authorId="3" shapeId="0" xr:uid="{E74B7E44-2395-6C42-B73D-2EC1F22A60C7}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Check these</t>
+      </text>
+    </comment>
+    <comment ref="G13" authorId="4" shapeId="0" xr:uid="{E9B3D22A-D92F-42DF-B73C-1C78227D06FF}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    PBK cut off dates</t>
+      </text>
+    </comment>
+    <comment ref="J13" authorId="5" shapeId="0" xr:uid="{A83E3842-9BE6-4EA3-92B3-E3B0D5967A00}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    PBK cut off dates</t>
       </text>
     </comment>
   </commentList>
@@ -73,15 +110,343 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={7DCF18E1-94DA-554A-8653-1E79DC5E2D8B}</author>
+    <author>tc={A724241D-7EDF-4998-98C9-2538634580EC}</author>
+    <author>tc={21C2CC1F-F6D3-4ADE-8907-C8066F843B52}</author>
+    <author>tc={BE139627-6C87-49E6-8EE2-CCDFEFDB54F3}</author>
+    <author>tc={524AD620-E4DF-45FF-AA62-4236DEF0A5B7}</author>
+    <author>tc={79C8CFB2-F2A5-4961-BE95-42938AB369FF}</author>
   </authors>
   <commentList>
-    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{7DCF18E1-94DA-554A-8653-1E79DC5E2D8B}">
+    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{A724241D-7EDF-4998-98C9-2538634580EC}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Omitting for now, because there’s no  scale information in the files. Change back to : 2014-03-27 01:18</t>
+    Overlap is not good.</t>
+      </text>
+    </comment>
+    <comment ref="D9" authorId="1" shapeId="0" xr:uid="{21C2CC1F-F6D3-4ADE-8907-C8066F843B52}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Overlap is not good.</t>
+      </text>
+    </comment>
+    <comment ref="C13" authorId="2" shapeId="0" xr:uid="{BE139627-6C87-49E6-8EE2-CCDFEFDB54F3}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Overlap is not good.</t>
+      </text>
+    </comment>
+    <comment ref="D13" authorId="3" shapeId="0" xr:uid="{524AD620-E4DF-45FF-AA62-4236DEF0A5B7}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Overlap is not good.</t>
+      </text>
+    </comment>
+    <comment ref="D15" authorId="4" shapeId="0" xr:uid="{79C8CFB2-F2A5-4961-BE95-42938AB369FF}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Data before too high.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={4B150629-4A57-4483-9656-9CE870FC0AC7}</author>
+    <author>tc={C7A463C2-EAF2-446F-895E-1E0F5EC9A2AE}</author>
+    <author>tc={0B781955-C493-4EB0-B776-F61E2EDAFE7B}</author>
+    <author>tc={40957B09-F877-4F7E-89B9-62E0202FECC7}</author>
+  </authors>
+  <commentList>
+    <comment ref="E11" authorId="0" shapeId="0" xr:uid="{4B150629-4A57-4483-9656-9CE870FC0AC7}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    PBK cut off dates</t>
+      </text>
+    </comment>
+    <comment ref="H11" authorId="1" shapeId="0" xr:uid="{C7A463C2-EAF2-446F-895E-1E0F5EC9A2AE}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    PBK cut off dates</t>
+      </text>
+    </comment>
+    <comment ref="E12" authorId="2" shapeId="0" xr:uid="{0B781955-C493-4EB0-B776-F61E2EDAFE7B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    PBK cut off dates</t>
+      </text>
+    </comment>
+    <comment ref="H12" authorId="3" shapeId="0" xr:uid="{40957B09-F877-4F7E-89B9-62E0202FECC7}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    PBK cut off dates</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={A47CBF8E-9E43-4C83-8A13-76A959DEE68D}</author>
+    <author>tc={CE1E1AA0-0B1C-48F3-8337-5F67189C3BCB}</author>
+    <author>tc={808642FA-BBFA-40BE-8C16-90EC1AC67A9C}</author>
+    <author>tc={43CCF54F-4E86-4E84-A9D1-21D4B69A1086}</author>
+  </authors>
+  <commentList>
+    <comment ref="G11" authorId="0" shapeId="0" xr:uid="{A47CBF8E-9E43-4C83-8A13-76A959DEE68D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    PBK cut off dates</t>
+      </text>
+    </comment>
+    <comment ref="H11" authorId="1" shapeId="0" xr:uid="{CE1E1AA0-0B1C-48F3-8337-5F67189C3BCB}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    PBK cut off dates</t>
+      </text>
+    </comment>
+    <comment ref="G12" authorId="2" shapeId="0" xr:uid="{808642FA-BBFA-40BE-8C16-90EC1AC67A9C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    PBK cut off dates</t>
+      </text>
+    </comment>
+    <comment ref="H12" authorId="3" shapeId="0" xr:uid="{43CCF54F-4E86-4E84-A9D1-21D4B69A1086}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    PBK cut off dates</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={52CD2559-4401-4986-9280-44FFB4BB19D9}</author>
+    <author>tc={C9F5E4D0-10CD-48F7-ADC2-63DAD41C55E3}</author>
+    <author>tc={60D4152A-579E-4866-B015-10E31354B64E}</author>
+    <author>tc={51C448EF-DA1A-460C-AB56-91B70D89FCBF}</author>
+    <author>tc={11D5FBC9-79F1-4079-ADB1-B04DC39E0766}</author>
+    <author>tc={044070EC-F2FD-4B5B-BA9E-AC62516EC883}</author>
+    <author>tc={5C85AD3E-D72C-4145-B7F2-4CE5A8A2A25E}</author>
+    <author>tc={A065C0A9-039C-43EE-BD11-3744606A6D5D}</author>
+    <author>tc={001B5564-298C-45EB-A10F-D8E085D2698D}</author>
+    <author>tc={C4E90346-FA53-4635-B45B-276088110233}</author>
+  </authors>
+  <commentList>
+    <comment ref="H9" authorId="0" shapeId="0" xr:uid="{52CD2559-4401-4986-9280-44FFB4BB19D9}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    # Medusa CFC-11 not compatible with MD CFC-11</t>
+      </text>
+    </comment>
+    <comment ref="H10" authorId="1" shapeId="0" xr:uid="{C9F5E4D0-10CD-48F7-ADC2-63DAD41C55E3}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    # No MD measurements since 2019-11-18 07:00. Medusa OK.</t>
+      </text>
+    </comment>
+    <comment ref="G11" authorId="2" shapeId="0" xr:uid="{60D4152A-579E-4866-B015-10E31354B64E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    PBK cut off dates</t>
+      </text>
+    </comment>
+    <comment ref="H11" authorId="3" shapeId="0" xr:uid="{51C448EF-DA1A-460C-AB56-91B70D89FCBF}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    PBK cut off dates</t>
+      </text>
+    </comment>
+    <comment ref="G12" authorId="4" shapeId="0" xr:uid="{11D5FBC9-79F1-4079-ADB1-B04DC39E0766}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    PBK cut off dates</t>
+      </text>
+    </comment>
+    <comment ref="H12" authorId="5" shapeId="0" xr:uid="{044070EC-F2FD-4B5B-BA9E-AC62516EC883}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    PBK cut off dates</t>
+      </text>
+    </comment>
+    <comment ref="H13" authorId="6" shapeId="0" xr:uid="{5C85AD3E-D72C-4145-B7F2-4CE5A8A2A25E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    # Medusa CCl4 not compatible with MD CCl4</t>
+      </text>
+    </comment>
+    <comment ref="H14" authorId="7" shapeId="0" xr:uid="{A065C0A9-039C-43EE-BD11-3744606A6D5D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    # No MD measurements since 2019-11-18 07:00</t>
+      </text>
+    </comment>
+    <comment ref="H15" authorId="8" shapeId="0" xr:uid="{001B5564-298C-45EB-A10F-D8E085D2698D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    # No MD measurements since 2019-11-18 07:00</t>
+      </text>
+    </comment>
+    <comment ref="H16" authorId="9" shapeId="0" xr:uid="{C4E90346-FA53-4635-B45B-276088110233}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    # No MD measurements since 2019-11-18 07:00. Medusa OK.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={DC673F18-F08F-4352-875B-E3DB87288217}</author>
+    <author>tc={7DCF18E1-94DA-554A-8653-1E79DC5E2D8B}</author>
+    <author>tc={FEF07E2C-6250-424E-B624-A7C0F271D8A8}</author>
+    <author>tc={D7FA52D0-B051-4A77-8D2B-D9401825D70E}</author>
+    <author>tc={6CD811DF-EA6C-4C89-9C00-A83A2889B66D}</author>
+    <author>tc={48D1302D-BD9F-474F-97EE-A5240196BBE3}</author>
+    <author>tc={0D6DDCEF-3D3B-4459-95EF-B4880811E75E}</author>
+    <author>tc={6155A2F0-F34E-4740-A077-90B2F6B19C5F}</author>
+    <author>tc={7DD994B2-D2E1-48E8-8EEC-577C9BB986DB}</author>
+    <author>tc={83C8BF56-4EA7-4376-9FF8-33698BC2A66E}</author>
+  </authors>
+  <commentList>
+    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{DC673F18-F08F-4352-875B-E3DB87288217}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Omitting for now, because there’s no  scale information in the files. Change back to : 2014-03-27 01:18
+Reply:
+    Changed to when the MD CH4 channel died (later fixed, but currently there can only be one cut off date). MD and Picarro are on different scales. Difference MD and Picarro is ~0.001 ppb. Ratio does not plot in GCCompare. </t>
+      </text>
+    </comment>
+    <comment ref="F9" authorId="1" shapeId="0" xr:uid="{7DCF18E1-94DA-554A-8653-1E79DC5E2D8B}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Omitting for now, because there’s no  scale information in the files. Change back to : 2014-03-27 01:18
+Reply:
+    Changed to when the MD CH4 channel died (later fixed, but currently there can only be one cut off date). MD and Picarro are on difference scales. Difference MD and Picarro is only ~0.001 ppb. Ratio does not plot in GCCompare. </t>
+      </text>
+    </comment>
+    <comment ref="C10" authorId="2" shapeId="0" xr:uid="{FEF07E2C-6250-424E-B624-A7C0F271D8A8}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    # PBK cut off dates</t>
+      </text>
+    </comment>
+    <comment ref="D10" authorId="3" shapeId="0" xr:uid="{D7FA52D0-B051-4A77-8D2B-D9401825D70E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    # PBK cut off dates# PBK cut off dates</t>
+      </text>
+    </comment>
+    <comment ref="C11" authorId="4" shapeId="0" xr:uid="{6CD811DF-EA6C-4C89-9C00-A83A2889B66D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    # PBK cut off dates</t>
+      </text>
+    </comment>
+    <comment ref="D11" authorId="5" shapeId="0" xr:uid="{48D1302D-BD9F-474F-97EE-A5240196BBE3}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    # PBK cut off dates</t>
+      </text>
+    </comment>
+    <comment ref="D12" authorId="6" shapeId="0" xr:uid="{0D6DDCEF-3D3B-4459-95EF-B4880811E75E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Use MD</t>
+      </text>
+    </comment>
+    <comment ref="D13" authorId="7" shapeId="0" xr:uid="{6155A2F0-F34E-4740-A077-90B2F6B19C5F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Use MD</t>
+      </text>
+    </comment>
+    <comment ref="D14" authorId="8" shapeId="0" xr:uid="{7DD994B2-D2E1-48E8-8EEC-577C9BB986DB}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Use MD</t>
+      </text>
+    </comment>
+    <comment ref="D15" authorId="9" shapeId="0" xr:uid="{83C8BF56-4EA7-4376-9FF8-33698BC2A66E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Use MD</t>
       </text>
     </comment>
   </commentList>
@@ -89,7 +454,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="94">
   <si>
     <t># File specifying when to use the various ALE/GAGE/AGAGE instruments</t>
   </si>
@@ -244,33 +609,18 @@
     <t>2003-11-15 16:50</t>
   </si>
   <si>
-    <t>2014-03-27 01:18</t>
-  </si>
-  <si>
     <t>2012-05-16 00:00</t>
   </si>
   <si>
     <t>2011-07-01 00:00</t>
   </si>
   <si>
-    <t>2010-11-30 00:00</t>
-  </si>
-  <si>
-    <t>2014-06-30 00:00</t>
-  </si>
-  <si>
     <t>1985-10-28 21:15</t>
   </si>
   <si>
     <t>1985-08-13 16:36</t>
   </si>
   <si>
-    <t>2005-07-31 00:00</t>
-  </si>
-  <si>
-    <t>2010-10-31 00:00</t>
-  </si>
-  <si>
     <t>2017-02-15 00:00</t>
   </si>
   <si>
@@ -283,9 +633,6 @@
     <t>1996-08-18 00:00</t>
   </si>
   <si>
-    <t>2006-05-28 03:12</t>
-  </si>
-  <si>
     <t>2010-09-02 00:00</t>
   </si>
   <si>
@@ -302,6 +649,93 @@
   </si>
   <si>
     <t>GCMS-MteCimone start</t>
+  </si>
+  <si>
+    <t>2011-01-01 00:00</t>
+  </si>
+  <si>
+    <t>2010-11-01 00:00</t>
+  </si>
+  <si>
+    <t>2005-08-01 00:00</t>
+  </si>
+  <si>
+    <t>2010-12-01 00:00</t>
+  </si>
+  <si>
+    <t>2019-11-18 07:00</t>
+  </si>
+  <si>
+    <t>2019-10-17 00:00</t>
+  </si>
+  <si>
+    <t>1985-11-01 00:00</t>
+  </si>
+  <si>
+    <t>1984-05-10 00:00</t>
+  </si>
+  <si>
+    <t>2023-12-20 00:47</t>
+  </si>
+  <si>
+    <t>2023-12-20 00:48</t>
+  </si>
+  <si>
+    <t>2023-12-20 00:49</t>
+  </si>
+  <si>
+    <t>2023-12-20 00:50</t>
+  </si>
+  <si>
+    <t>2023-12-20 00:51</t>
+  </si>
+  <si>
+    <t>2023-12-20 00:52</t>
+  </si>
+  <si>
+    <t>2023-12-20 00:53</t>
+  </si>
+  <si>
+    <t>2023-12-20 00:54</t>
+  </si>
+  <si>
+    <t>2023-12-20 00:55</t>
+  </si>
+  <si>
+    <t>2023-12-20 00:56</t>
+  </si>
+  <si>
+    <t>2023-12-20 00:57</t>
+  </si>
+  <si>
+    <t>2023-12-20 00:58</t>
+  </si>
+  <si>
+    <t>2023-12-20 00:59</t>
+  </si>
+  <si>
+    <t>2023-12-20 00:60</t>
+  </si>
+  <si>
+    <t>2023-12-20 00:61</t>
+  </si>
+  <si>
+    <t>2016-09-02 21:00</t>
+  </si>
+  <si>
+    <t>co</t>
+  </si>
+  <si>
+    <t>2018-03-14 00:00</t>
+  </si>
+  <si>
+    <t>sf6</t>
+  </si>
+  <si>
+    <t>LGR end</t>
+  </si>
+  <si>
+    <t>LGR start</t>
   </si>
 </sst>
 </file>
@@ -331,8 +765,10 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
+      <i/>
       <sz val="12"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -395,14 +831,15 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Muhle, Jens" id="{45642C69-8A44-412F-9E7D-D9558092E6B7}" userId="S::jmuhle@UCSD.EDU::0abe738f-e9aa-4c03-a4a8-7d5d29529c36" providerId="AD"/>
   <person displayName="Matthew Rigby" id="{34B736E8-4CAD-3843-A1A8-25F59C5B220F}" userId="S::chxmr@bristol.ac.uk::ca6cd915-32ac-44b1-8565-a73cfd7038de" providerId="AD"/>
 </personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -440,7 +877,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -546,7 +983,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -688,7 +1125,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -699,16 +1136,150 @@
   <threadedComment ref="E9" dT="2023-07-22T05:26:38.42" personId="{34B736E8-4CAD-3843-A1A8-25F59C5B220F}" id="{E2A43AB0-C9B5-4349-922D-876081C672EC}">
     <text>I just made these CH4 dates up for testing</text>
   </threadedComment>
+  <threadedComment ref="G10" dT="2024-05-16T18:37:31.91" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{E55AD725-15DB-43AB-8E3D-FF58A480B65B}">
+    <text>PBK cut off dates</text>
+  </threadedComment>
+  <threadedComment ref="J10" dT="2024-05-16T18:37:40.22" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{5540EEFA-5767-4C3A-97E4-DDFAA77A7BDD}">
+    <text>PBK cut off dates</text>
+  </threadedComment>
   <threadedComment ref="C11" dT="2023-07-26T20:04:11.42" personId="{34B736E8-4CAD-3843-A1A8-25F59C5B220F}" id="{E74B7E44-2395-6C42-B73D-2EC1F22A60C7}">
     <text>Check these</text>
+  </threadedComment>
+  <threadedComment ref="G13" dT="2024-05-16T18:37:35.57" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{E9B3D22A-D92F-42DF-B73C-1C78227D06FF}">
+    <text>PBK cut off dates</text>
+  </threadedComment>
+  <threadedComment ref="J13" dT="2024-05-16T18:37:43.80" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{A83E3842-9BE6-4EA3-92B3-E3B0D5967A00}">
+    <text>PBK cut off dates</text>
   </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="C9" dT="2024-05-21T23:22:15.56" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{A724241D-7EDF-4998-98C9-2538634580EC}">
+    <text>Overlap is not good.</text>
+  </threadedComment>
+  <threadedComment ref="D9" dT="2024-05-21T23:22:21.69" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{21C2CC1F-F6D3-4ADE-8907-C8066F843B52}">
+    <text>Overlap is not good.</text>
+  </threadedComment>
+  <threadedComment ref="C13" dT="2024-05-21T23:21:56.37" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{BE139627-6C87-49E6-8EE2-CCDFEFDB54F3}">
+    <text>Overlap is not good.</text>
+  </threadedComment>
+  <threadedComment ref="D13" dT="2024-05-21T23:22:05.51" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{524AD620-E4DF-45FF-AA62-4236DEF0A5B7}">
+    <text>Overlap is not good.</text>
+  </threadedComment>
+  <threadedComment ref="D15" dT="2024-05-21T23:22:54.53" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{79C8CFB2-F2A5-4961-BE95-42938AB369FF}">
+    <text>Data before too high.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="E11" dT="2024-05-16T18:37:21.53" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{4B150629-4A57-4483-9656-9CE870FC0AC7}">
+    <text>PBK cut off dates</text>
+  </threadedComment>
+  <threadedComment ref="H11" dT="2024-05-16T18:37:08.61" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{C7A463C2-EAF2-446F-895E-1E0F5EC9A2AE}">
+    <text>PBK cut off dates</text>
+  </threadedComment>
+  <threadedComment ref="E12" dT="2024-05-16T18:37:25.44" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{0B781955-C493-4EB0-B776-F61E2EDAFE7B}">
+    <text>PBK cut off dates</text>
+  </threadedComment>
+  <threadedComment ref="H12" dT="2024-05-16T18:37:14.70" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{40957B09-F877-4F7E-89B9-62E0202FECC7}">
+    <text>PBK cut off dates</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment4.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="G11" dT="2024-05-16T18:37:54.14" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{A47CBF8E-9E43-4C83-8A13-76A959DEE68D}">
+    <text>PBK cut off dates</text>
+  </threadedComment>
+  <threadedComment ref="H11" dT="2024-05-16T18:38:01.07" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{CE1E1AA0-0B1C-48F3-8337-5F67189C3BCB}">
+    <text>PBK cut off dates</text>
+  </threadedComment>
+  <threadedComment ref="G12" dT="2024-05-16T18:37:57.47" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{808642FA-BBFA-40BE-8C16-90EC1AC67A9C}">
+    <text>PBK cut off dates</text>
+  </threadedComment>
+  <threadedComment ref="H12" dT="2024-05-16T18:38:08.20" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{43CCF54F-4E86-4E84-A9D1-21D4B69A1086}">
+    <text>PBK cut off dates</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment5.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="H9" dT="2024-05-16T18:39:12.60" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{52CD2559-4401-4986-9280-44FFB4BB19D9}">
+    <text># Medusa CFC-11 not compatible with MD CFC-11</text>
+  </threadedComment>
+  <threadedComment ref="H10" dT="2024-05-16T18:39:03.32" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{C9F5E4D0-10CD-48F7-ADC2-63DAD41C55E3}">
+    <text># No MD measurements since 2019-11-18 07:00. Medusa OK.</text>
+  </threadedComment>
+  <threadedComment ref="G11" dT="2024-05-16T18:38:19.20" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{60D4152A-579E-4866-B015-10E31354B64E}">
+    <text>PBK cut off dates</text>
+  </threadedComment>
+  <threadedComment ref="H11" dT="2024-05-16T18:38:26.92" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{51C448EF-DA1A-460C-AB56-91B70D89FCBF}">
+    <text>PBK cut off dates</text>
+  </threadedComment>
+  <threadedComment ref="G12" dT="2024-05-16T18:38:22.87" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{11D5FBC9-79F1-4079-ADB1-B04DC39E0766}">
+    <text>PBK cut off dates</text>
+  </threadedComment>
+  <threadedComment ref="H12" dT="2024-05-16T18:38:30.65" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{044070EC-F2FD-4B5B-BA9E-AC62516EC883}">
+    <text>PBK cut off dates</text>
+  </threadedComment>
+  <threadedComment ref="H13" dT="2024-05-16T18:38:39.19" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{5C85AD3E-D72C-4145-B7F2-4CE5A8A2A25E}">
+    <text># Medusa CCl4 not compatible with MD CCl4</text>
+  </threadedComment>
+  <threadedComment ref="H14" dT="2024-05-16T18:38:48.53" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{A065C0A9-039C-43EE-BD11-3744606A6D5D}">
+    <text># No MD measurements since 2019-11-18 07:00</text>
+  </threadedComment>
+  <threadedComment ref="H15" dT="2024-05-16T18:38:53.61" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{001B5564-298C-45EB-A10F-D8E085D2698D}">
+    <text># No MD measurements since 2019-11-18 07:00</text>
+  </threadedComment>
+  <threadedComment ref="H16" dT="2024-05-16T18:39:03.32" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{C4E90346-FA53-4635-B45B-276088110233}">
+    <text># No MD measurements since 2019-11-18 07:00. Medusa OK.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment6.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="C9" dT="2023-08-03T19:20:56.95" personId="{34B736E8-4CAD-3843-A1A8-25F59C5B220F}" id="{DC673F18-F08F-4352-875B-E3DB87288217}">
+    <text>Omitting for now, because there’s no  scale information in the files. Change back to : 2014-03-27 01:18</text>
+  </threadedComment>
+  <threadedComment ref="C9" dT="2024-05-16T20:50:40.64" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{E78EA206-A2C1-4B7B-A09C-6C314C04B95C}" parentId="{DC673F18-F08F-4352-875B-E3DB87288217}">
+    <text xml:space="preserve">Changed to when the MD CH4 channel died (later fixed, but currently there can only be one cut off date). MD and Picarro are on different scales. Difference MD and Picarro is ~0.001 ppb. Ratio does not plot in GCCompare. </text>
+  </threadedComment>
   <threadedComment ref="F9" dT="2023-08-03T19:20:56.95" personId="{34B736E8-4CAD-3843-A1A8-25F59C5B220F}" id="{7DCF18E1-94DA-554A-8653-1E79DC5E2D8B}">
     <text>Omitting for now, because there’s no  scale information in the files. Change back to : 2014-03-27 01:18</text>
+  </threadedComment>
+  <threadedComment ref="F9" dT="2024-05-16T20:50:40.64" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{FE1930E4-AC0F-4ECB-A34F-66EE9640FFE9}" parentId="{7DCF18E1-94DA-554A-8653-1E79DC5E2D8B}">
+    <text xml:space="preserve">Changed to when the MD CH4 channel died (later fixed, but currently there can only be one cut off date). MD and Picarro are on difference scales. Difference MD and Picarro is only ~0.001 ppb. Ratio does not plot in GCCompare. </text>
+  </threadedComment>
+  <threadedComment ref="C10" dT="2024-05-16T18:41:38.90" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{FEF07E2C-6250-424E-B624-A7C0F271D8A8}">
+    <text># PBK cut off dates</text>
+  </threadedComment>
+  <threadedComment ref="D10" dT="2024-05-16T18:35:47.81" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{D7FA52D0-B051-4A77-8D2B-D9401825D70E}">
+    <text># PBK cut off dates# PBK cut off dates</text>
+  </threadedComment>
+  <threadedComment ref="C11" dT="2024-05-16T18:41:42.76" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{6CD811DF-EA6C-4C89-9C00-A83A2889B66D}">
+    <text># PBK cut off dates</text>
+  </threadedComment>
+  <threadedComment ref="D11" dT="2024-05-16T18:36:03.42" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{48D1302D-BD9F-474F-97EE-A5240196BBE3}">
+    <text># PBK cut off dates</text>
+  </threadedComment>
+  <threadedComment ref="D12" dT="2024-05-16T18:36:16.10" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{0D6DDCEF-3D3B-4459-95EF-B4880811E75E}">
+    <text>Use MD</text>
+  </threadedComment>
+  <threadedComment ref="D13" dT="2024-05-16T18:36:42.42" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{6155A2F0-F34E-4740-A077-90B2F6B19C5F}">
+    <text>Use MD</text>
+  </threadedComment>
+  <threadedComment ref="D14" dT="2024-05-16T18:36:47.23" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{7DD994B2-D2E1-48E8-8EEC-577C9BB986DB}">
+    <text>Use MD</text>
+  </threadedComment>
+  <threadedComment ref="D15" dT="2024-05-16T18:36:51.82" personId="{45642C69-8A44-412F-9E7D-D9558092E6B7}" id="{83C8BF56-4EA7-4376-9FF8-33698BC2A66E}">
+    <text>Use MD</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -718,10 +1289,10 @@
   <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="1"/>
     <col min="3" max="3" width="15.5" style="1" bestFit="1" customWidth="1"/>
@@ -861,7 +1432,7 @@
       <c r="F10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="2" t="s">
         <v>18</v>
       </c>
       <c r="H10" s="1" t="s">
@@ -870,7 +1441,7 @@
       <c r="I10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" s="2" t="s">
         <v>18</v>
       </c>
       <c r="L10" s="1" t="s">
@@ -969,14 +1540,17 @@
       <c r="F13" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="G13" s="5" t="s">
+        <v>65</v>
+      </c>
       <c r="H13" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>15</v>
+      <c r="J13" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>15</v>
@@ -1554,15 +2128,484 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C42BA6F3-6164-0740-9787-95981F3E2AF1}">
+  <dimension ref="A1:I22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02AF7775-65E2-7E48-BA80-42F8CA71CBFC}">
-  <dimension ref="A1:I13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{282330B1-5456-C947-8C60-CDB83BC163C1}">
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="20.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02AF7775-65E2-7E48-BA80-42F8CA71CBFC}">
+  <dimension ref="A1:I15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="1"/>
     <col min="3" max="3" width="15.5" style="1" bestFit="1" customWidth="1"/>
@@ -1626,10 +2669,10 @@
       <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1637,10 +2680,10 @@
       <c r="A10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1648,10 +2691,10 @@
       <c r="A11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1659,10 +2702,10 @@
       <c r="A12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1670,11 +2713,257 @@
       <c r="A13" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="C13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE54F353-AB0A-D84A-B024-6541A31A2D76}">
+  <dimension ref="A1:I22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="C13" s="1" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>16</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1682,15 +2971,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC29711F-13B8-9140-B473-D8767E35D5EB}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC29711F-13B8-9140-B473-D8767E35D5EB}">
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="O11" sqref="O11:O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="5" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
@@ -1840,8 +3129,8 @@
       <c r="D11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>54</v>
+      <c r="E11" s="5" t="s">
+        <v>68</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>15</v>
@@ -1850,7 +3139,7 @@
         <v>15</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>15</v>
@@ -1869,8 +3158,8 @@
       <c r="D12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>55</v>
+      <c r="E12" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>15</v>
@@ -1878,8 +3167,8 @@
       <c r="G12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>55</v>
+      <c r="H12" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>15</v>
@@ -2378,141 +3667,6 @@
         <v>15</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{160591D1-02F5-5E4D-B7FE-18CBFE4B0D82}">
-  <dimension ref="A1:K11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="3" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="10.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2522,15 +3676,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95CA49D9-7FA7-1249-B393-DC69D0A3EC82}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95CA49D9-7FA7-1249-B393-DC69D0A3EC82}">
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="1"/>
     <col min="3" max="3" width="15.5" style="1" bestFit="1" customWidth="1"/>
@@ -2616,16 +3770,16 @@
         <v>28</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>15</v>
@@ -2645,16 +3799,16 @@
         <v>29</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>15</v>
@@ -2680,16 +3834,16 @@
         <v>15</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>67</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>15</v>
@@ -2703,22 +3857,22 @@
         <v>27</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>59</v>
+      <c r="G12" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>15</v>
@@ -2732,16 +3886,16 @@
         <v>30</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>15</v>
@@ -2761,16 +3915,16 @@
         <v>31</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>15</v>
@@ -2796,13 +3950,13 @@
         <v>15</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>15</v>
@@ -2811,23 +3965,24 @@
         <v>15</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C45BA512-5AE4-3C4F-BEFD-5BBCD1F01554}">
-  <dimension ref="A1:O15"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C45BA512-5AE4-3C4F-BEFD-5BBCD1F01554}">
+  <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="1"/>
     <col min="3" max="3" width="15.5" style="1" bestFit="1" customWidth="1"/>
@@ -2912,19 +4067,19 @@
       <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H9" s="1" t="s">
+      <c r="C9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I9" s="1" t="s">
@@ -2941,20 +4096,20 @@
       <c r="A10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>15</v>
+      <c r="C10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>69</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>15</v>
@@ -2976,17 +4131,17 @@
       <c r="C11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>64</v>
+      <c r="E11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>52</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>15</v>
@@ -2999,23 +4154,23 @@
       <c r="A12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>64</v>
+      <c r="C12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>15</v>
@@ -3028,19 +4183,19 @@
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H13" s="1" t="s">
+      <c r="C13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I13" s="1" t="s">
@@ -3057,17 +4212,17 @@
       <c r="A14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>63</v>
+      <c r="C14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>15</v>
@@ -3092,11 +4247,11 @@
       <c r="C15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>63</v>
+      <c r="E15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>15</v>
@@ -3108,305 +4263,110 @@
         <v>15</v>
       </c>
       <c r="K15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C42BA6F3-6164-0740-9787-95981F3E2AF1}">
-  <dimension ref="A1:I22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="14.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="10.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE54F353-AB0A-D84A-B024-6541A31A2D76}">
-  <dimension ref="A1:I22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BE17A77-6BC1-934F-9E75-E00D36D67A2D}">
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="14.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" style="1"/>
+    <col min="2" max="3" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="11.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>12</v>
@@ -3414,159 +4374,88 @@
       <c r="E8" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>34</v>
+      <c r="F8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>35</v>
+        <v>15</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>67</v>
+        <v>15</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>67</v>
+        <v>15</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>37</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>67</v>
+        <v>15</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -3575,67 +4464,67 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{282330B1-5456-C947-8C60-CDB83BC163C1}">
-  <dimension ref="A1:I23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{160591D1-02F5-5E4D-B7FE-18CBFE4B0D82}">
+  <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="20.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>69</v>
+        <v>10</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>12</v>
@@ -3643,173 +4532,115 @@
       <c r="E8" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>68</v>
+        <v>26</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O10" s="1"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>68</v>
+        <v>32</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O11" s="1"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>68</v>
+        <v>15</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed some CMN timestamps that don't exist
</commit_message>
<xml_diff>
--- a/data/agage/data_combination.xlsx
+++ b/data/agage/data_combination.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="CGO"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="92">
   <si>
     <t># File specifying when to use the various ALE/GAGE/AGAGE instruments</t>
   </si>
@@ -127,9 +127,6 @@
     <t>x</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>2012-05-16 00:00</t>
   </si>
   <si>
@@ -287,12 +284,6 @@
   </si>
   <si>
     <t>2023-12-20 00:59</t>
-  </si>
-  <si>
-    <t>2023-12-20 00:60</t>
-  </si>
-  <si>
-    <t>2023-12-20 00:61</t>
   </si>
   <si>
     <t>1994-01-01 00:00</t>
@@ -325,7 +316,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -395,6 +386,9 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -408,9 +402,6 @@
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -723,7 +714,7 @@
   </sheetPr>
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -734,10 +725,10 @@
     <col min="5" max="5" style="6" width="15.862142857142858" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="6" width="15.862142857142858" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="6" width="15.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="6" width="14.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="7" width="14.576428571428572" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="6" width="15.576428571428572" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="6" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="6" width="17.005" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="7" width="17.005" customWidth="1" bestFit="1"/>
     <col min="12" max="12" style="6" width="15.576428571428572" customWidth="1" bestFit="1"/>
     <col min="13" max="13" style="6" width="10.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
@@ -746,159 +737,159 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
       <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
       <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="K8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="L8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="M8" s="4" t="s">
         <v>30</v>
       </c>
     </row>
@@ -912,15 +903,15 @@
       <c r="C9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="3"/>
       <c r="E9" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>33</v>
@@ -935,29 +926,29 @@
         <v>33</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="M9" s="2"/>
+        <v>88</v>
+      </c>
+      <c r="M9" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="3"/>
       <c r="C10" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>90</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>33</v>
@@ -965,8 +956,8 @@
       <c r="I10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J10" s="3" t="s">
-        <v>93</v>
+      <c r="J10" s="4" t="s">
+        <v>90</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="1" t="s">
@@ -978,22 +969,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
       <c r="A11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="B11" s="3"/>
       <c r="C11" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G11" s="2"/>
+        <v>89</v>
+      </c>
+      <c r="G11" s="3"/>
       <c r="H11" s="1" t="s">
         <v>33</v>
       </c>
@@ -1015,22 +1006,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
       <c r="A12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="B12" s="3"/>
       <c r="C12" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G12" s="2"/>
+        <v>89</v>
+      </c>
+      <c r="G12" s="3"/>
       <c r="H12" s="1" t="s">
         <v>33</v>
       </c>
@@ -1052,7 +1043,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>33</v>
@@ -1061,16 +1052,16 @@
         <v>33</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>55</v>
+        <v>89</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>33</v>
@@ -1078,8 +1069,8 @@
       <c r="I13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J13" s="7" t="s">
-        <v>55</v>
+      <c r="J13" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>33</v>
@@ -1093,22 +1084,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
       <c r="A14" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="B14" s="3"/>
       <c r="C14" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G14" s="2"/>
+        <v>89</v>
+      </c>
+      <c r="G14" s="3"/>
       <c r="H14" s="1" t="s">
         <v>33</v>
       </c>
@@ -1130,22 +1121,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
       <c r="A15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="B15" s="3"/>
       <c r="C15" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G15" s="2"/>
+        <v>89</v>
+      </c>
+      <c r="G15" s="3"/>
       <c r="H15" s="1" t="s">
         <v>33</v>
       </c>
@@ -1189,10 +1180,10 @@
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="1" t="s">
@@ -1226,10 +1217,10 @@
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K17" s="2"/>
       <c r="L17" s="1" t="s">
@@ -1263,10 +1254,10 @@
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K18" s="2"/>
       <c r="L18" s="1" t="s">
@@ -1300,10 +1291,10 @@
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K19" s="2"/>
       <c r="L19" s="1" t="s">
@@ -1337,10 +1328,10 @@
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K20" s="2"/>
       <c r="L20" s="1" t="s">
@@ -1374,10 +1365,10 @@
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K21" s="2"/>
       <c r="L21" s="1" t="s">
@@ -1411,10 +1402,10 @@
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K22" s="2"/>
       <c r="L22" s="1" t="s">
@@ -1448,10 +1439,10 @@
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K23" s="2"/>
       <c r="L23" s="1" t="s">
@@ -1485,10 +1476,10 @@
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K24" s="2"/>
       <c r="L24" s="1" t="s">
@@ -1522,10 +1513,10 @@
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K25" s="2"/>
       <c r="L25" s="1" t="s">
@@ -1559,10 +1550,10 @@
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K26" s="2"/>
       <c r="L26" s="1" t="s">
@@ -1596,10 +1587,10 @@
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K27" s="2"/>
       <c r="L27" s="1" t="s">
@@ -1633,10 +1624,10 @@
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K28" s="2"/>
       <c r="L28" s="1" t="s">
@@ -1648,7 +1639,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
       <c r="A29" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>33</v>
@@ -1670,10 +1661,10 @@
       </c>
       <c r="H29" s="2"/>
       <c r="I29" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K29" s="2"/>
       <c r="L29" s="1" t="s">
@@ -1699,11 +1690,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="14.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="14.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="6" width="15.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="6" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="17.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="17.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -1711,8 +1702,8 @@
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
       <c r="E1" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
@@ -1720,8 +1711,8 @@
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
       <c r="E2" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
@@ -1729,8 +1720,8 @@
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
       <c r="E3" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
@@ -1738,8 +1729,8 @@
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
       <c r="E4" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
@@ -1747,8 +1738,8 @@
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
       <c r="E5" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
@@ -1756,8 +1747,8 @@
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
       <c r="E6" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
@@ -1765,29 +1756,29 @@
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
       <c r="E7" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="2"/>
@@ -1800,7 +1791,7 @@
       <c r="E9" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="2"/>
@@ -1813,7 +1804,7 @@
       <c r="E10" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="2"/>
@@ -1826,7 +1817,7 @@
       <c r="E11" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="2"/>
@@ -1839,7 +1830,7 @@
       <c r="E12" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="2"/>
@@ -1852,7 +1843,7 @@
       <c r="E13" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="2"/>
@@ -1865,7 +1856,7 @@
       <c r="E14" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="2"/>
@@ -1878,7 +1869,7 @@
       <c r="E15" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="2"/>
@@ -1891,7 +1882,7 @@
       <c r="E16" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="2"/>
@@ -1904,7 +1895,7 @@
       <c r="E17" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="2"/>
@@ -1917,7 +1908,7 @@
       <c r="E18" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="2"/>
@@ -1930,7 +1921,7 @@
       <c r="E19" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="2"/>
@@ -1943,7 +1934,7 @@
       <c r="E20" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B21" s="2"/>
@@ -1956,7 +1947,7 @@
       <c r="E21" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B22" s="2"/>
@@ -1980,289 +1971,289 @@
   </sheetPr>
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="6" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="20.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="20.862142857142857" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="6" width="20.005" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="6" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="17.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="17.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
       <c r="E1" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
       <c r="E2" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
       <c r="E3" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
       <c r="E4" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
       <c r="E5" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
       <c r="E6" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
       <c r="E7" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
-      <c r="A8" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="E9" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E19" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E20" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E22" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E23" s="2"/>
     </row>
@@ -2283,10 +2274,10 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="6" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="15.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="15.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="6" width="15.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="15.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="15.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -2295,7 +2286,7 @@
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="D1" s="3"/>
       <c r="E1" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
@@ -2304,7 +2295,7 @@
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="D2" s="3"/>
       <c r="E2" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
@@ -2313,7 +2304,7 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="D3" s="3"/>
       <c r="E3" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
@@ -2322,7 +2313,7 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="D4" s="3"/>
       <c r="E4" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
@@ -2331,7 +2322,7 @@
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="D5" s="3"/>
       <c r="E5" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
@@ -2340,7 +2331,7 @@
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="D6" s="3"/>
       <c r="E6" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
@@ -2349,49 +2340,49 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="D7" s="3"/>
       <c r="E7" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>51</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
       <c r="A9" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>69</v>
+      <c r="C9" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="E9" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
       <c r="A10" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>69</v>
+      <c r="C10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="E10" s="2"/>
     </row>
@@ -2400,59 +2391,59 @@
         <v>26</v>
       </c>
       <c r="B11" s="2"/>
-      <c r="C11" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>69</v>
+      <c r="C11" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="E11" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
       <c r="A12" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" s="2"/>
-      <c r="C12" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>69</v>
+      <c r="C12" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="E12" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
       <c r="A13" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B13" s="2"/>
-      <c r="C13" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>69</v>
+      <c r="C13" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="E13" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="8" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="7" t="s">
-        <v>70</v>
+      <c r="D14" s="8" t="s">
+        <v>69</v>
       </c>
       <c r="E14" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
-      <c r="A15" s="7" t="s">
-        <v>36</v>
+      <c r="A15" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
-      <c r="D15" s="7" t="s">
-        <v>71</v>
+      <c r="D15" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="E15" s="2"/>
     </row>
@@ -2472,11 +2463,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="14.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="14.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="6" width="15.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="6" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="17.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="17.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -2484,8 +2475,8 @@
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
       <c r="E1" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
@@ -2493,8 +2484,8 @@
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
       <c r="E2" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
@@ -2502,8 +2493,8 @@
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
       <c r="E3" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
@@ -2511,8 +2502,8 @@
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
       <c r="E4" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
@@ -2520,8 +2511,8 @@
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
       <c r="E5" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
@@ -2529,8 +2520,8 @@
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
       <c r="E6" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
@@ -2538,206 +2529,206 @@
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
       <c r="E7" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E9" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E10" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E11" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E12" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E13" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E14" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E15" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E16" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E17" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E18" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E19" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
-      <c r="A20" s="4" t="s">
-        <v>65</v>
+      <c r="A20" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+      <c r="A21" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
-      <c r="A21" s="4" t="s">
-        <v>67</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E21" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
-      <c r="A22" s="4" t="s">
-        <v>68</v>
+      <c r="A22" s="5" t="s">
+        <v>67</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E22" s="2"/>
     </row>
@@ -2762,10 +2753,10 @@
     <col min="3" max="3" style="6" width="15.862142857142858" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="6" width="15.862142857142858" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="6" width="15.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="14.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="7" width="14.576428571428572" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="6" width="15.576428571428572" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="6" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="6" width="17.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="7" width="17.005" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="6" width="15.576428571428572" customWidth="1" bestFit="1"/>
     <col min="11" max="11" style="6" width="10.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
@@ -2774,154 +2765,154 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
       <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
       <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
       <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="K8" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
       <c r="A9" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="B9" s="3"/>
       <c r="C9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E9" s="2"/>
+        <v>61</v>
+      </c>
+      <c r="E9" s="3"/>
       <c r="F9" s="1" t="s">
         <v>33</v>
       </c>
@@ -2943,16 +2934,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
       <c r="A10" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="B10" s="3"/>
       <c r="C10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" s="2"/>
+        <v>61</v>
+      </c>
+      <c r="E10" s="3"/>
       <c r="F10" s="1" t="s">
         <v>33</v>
       </c>
@@ -2974,26 +2965,26 @@
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
       <c r="A11" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="B11" s="3"/>
       <c r="C11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="F11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="8" t="s">
         <v>62</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>63</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="1" t="s">
@@ -3007,15 +2998,15 @@
       <c r="A12" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="3"/>
       <c r="C12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>55</v>
+        <v>61</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>33</v>
@@ -3023,8 +3014,8 @@
       <c r="G12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="7" t="s">
-        <v>55</v>
+      <c r="H12" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="1" t="s">
@@ -3036,16 +3027,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
       <c r="A13" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="B13" s="3"/>
       <c r="C13" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E13" s="2"/>
+        <v>61</v>
+      </c>
+      <c r="E13" s="3"/>
       <c r="F13" s="1" t="s">
         <v>33</v>
       </c>
@@ -3067,16 +3058,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
       <c r="A14" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="B14" s="3"/>
       <c r="C14" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E14" s="2"/>
+        <v>61</v>
+      </c>
+      <c r="E14" s="3"/>
       <c r="F14" s="1" t="s">
         <v>33</v>
       </c>
@@ -3100,14 +3091,14 @@
       <c r="A15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="3"/>
       <c r="C15" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E15" s="2"/>
+        <v>61</v>
+      </c>
+      <c r="E15" s="3"/>
       <c r="F15" s="1" t="s">
         <v>33</v>
       </c>
@@ -3145,10 +3136,10 @@
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="1" t="s">
@@ -3176,10 +3167,10 @@
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="1" t="s">
@@ -3207,10 +3198,10 @@
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="1" t="s">
@@ -3238,10 +3229,10 @@
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="1" t="s">
@@ -3269,10 +3260,10 @@
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="1" t="s">
@@ -3300,10 +3291,10 @@
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="1" t="s">
@@ -3331,10 +3322,10 @@
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="1" t="s">
@@ -3362,10 +3353,10 @@
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="1" t="s">
@@ -3393,10 +3384,10 @@
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="1" t="s">
@@ -3424,10 +3415,10 @@
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="1" t="s">
@@ -3455,10 +3446,10 @@
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="1" t="s">
@@ -3486,10 +3477,10 @@
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="1" t="s">
@@ -3517,10 +3508,10 @@
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="1" t="s">
@@ -3532,7 +3523,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
       <c r="A29" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>33</v>
@@ -3548,10 +3539,10 @@
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="1" t="s">
@@ -3580,174 +3571,174 @@
     <col min="1" max="1" style="6" width="10.862142857142858" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="6" width="10.862142857142858" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="6" width="15.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="15.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="15.862142857142858" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="6" width="15.862142857142858" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="6" width="15.862142857142858" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="6" width="15.862142857142858" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="6" width="17.862142857142857" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="6" width="17.005" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="6" width="15.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="6" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="7" width="10.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
       <c r="K1" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
       <c r="K2" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
       <c r="K3" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
       <c r="K4" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
       <c r="K5" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
       <c r="K6" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
       <c r="K7" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="K8" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
       <c r="A9" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="B9" s="3"/>
       <c r="C9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G9" s="2"/>
+      <c r="G9" s="3"/>
       <c r="H9" s="1" t="s">
         <v>33</v>
       </c>
@@ -3763,22 +3754,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
       <c r="A10" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="B10" s="3"/>
       <c r="C10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G10" s="2"/>
+      <c r="G10" s="3"/>
       <c r="H10" s="1" t="s">
         <v>33</v>
       </c>
@@ -3794,7 +3785,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
       <c r="A11" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>33</v>
@@ -3804,18 +3795,18 @@
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="H11" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="G11" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="I11" s="2"/>
+      <c r="I11" s="3"/>
       <c r="J11" s="1" t="s">
         <v>33</v>
       </c>
@@ -3827,26 +3818,26 @@
       <c r="A12" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="3"/>
       <c r="C12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="H12" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="I12" s="2"/>
+      <c r="I12" s="3"/>
       <c r="J12" s="1" t="s">
         <v>33</v>
       </c>
@@ -3856,22 +3847,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
       <c r="A13" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="B13" s="3"/>
       <c r="C13" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G13" s="2"/>
+        <v>56</v>
+      </c>
+      <c r="G13" s="3"/>
       <c r="H13" s="1" t="s">
         <v>33</v>
       </c>
@@ -3887,22 +3878,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
       <c r="A14" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="B14" s="3"/>
       <c r="C14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G14" s="2"/>
+      <c r="G14" s="3"/>
       <c r="H14" s="1" t="s">
         <v>33</v>
       </c>
@@ -3928,13 +3919,13 @@
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>33</v>
@@ -3943,7 +3934,7 @@
         <v>33</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K15" s="2"/>
     </row>
@@ -3969,7 +3960,7 @@
     <col min="4" max="4" style="6" width="15.862142857142858" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="6" width="15.862142857142858" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="6" width="15.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="6" width="15.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="7" width="15.862142857142858" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="6" width="17.862142857142857" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="6" width="17.005" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="6" width="15.576428571428572" customWidth="1" bestFit="1"/>
@@ -3980,161 +3971,161 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
       <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="K8" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
       <c r="A9" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="F9" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="G9" s="2"/>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="4" t="s">
         <v>33</v>
       </c>
       <c r="I9" s="1" t="s">
@@ -4149,24 +4140,24 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
       <c r="A10" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="F10" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="G10" s="2"/>
+      <c r="H10" s="8" t="s">
         <v>53</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="7" t="s">
-        <v>54</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>33</v>
@@ -4180,28 +4171,28 @@
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
       <c r="A11" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="I11" s="2"/>
+      <c r="H11" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I11" s="3"/>
       <c r="J11" s="1" t="s">
         <v>33</v>
       </c>
@@ -4213,26 +4204,26 @@
       <c r="A12" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="3" t="s">
+      <c r="B12" s="3"/>
+      <c r="C12" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="F12" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="I12" s="2"/>
+      <c r="G12" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" s="3"/>
       <c r="J12" s="1" t="s">
         <v>33</v>
       </c>
@@ -4242,23 +4233,23 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
       <c r="A13" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="F13" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="G13" s="2"/>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="4" t="s">
         <v>33</v>
       </c>
       <c r="I13" s="1" t="s">
@@ -4273,20 +4264,20 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
       <c r="A14" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="F14" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="1" t="s">
@@ -4312,12 +4303,12 @@
       <c r="C15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>53</v>
+      <c r="D15" s="3"/>
+      <c r="E15" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="1" t="s">
@@ -4349,12 +4340,12 @@
       <c r="E16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="8" t="s">
         <v>53</v>
-      </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="7" t="s">
-        <v>54</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>33</v>
@@ -4383,14 +4374,14 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="6" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="15.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="15.862142857142858" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="6" width="15.862142857142858" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="6" width="17.862142857142857" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="6" width="17.005" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="6" width="15.576428571428572" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="6" width="11.147857142857141" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="6" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="6" width="11.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="7" width="11.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -4398,12 +4389,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
       <c r="I1" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
@@ -4411,12 +4402,12 @@
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
       <c r="I2" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
@@ -4424,12 +4415,12 @@
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
       <c r="I3" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
@@ -4437,12 +4428,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
       <c r="I4" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
@@ -4450,12 +4441,12 @@
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
       <c r="I5" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
@@ -4463,12 +4454,12 @@
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
       <c r="I6" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
@@ -4476,50 +4467,50 @@
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
       <c r="I7" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
       <c r="A9" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>33</v>
@@ -4534,7 +4525,7 @@
         <v>33</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I9" s="2"/>
     </row>
@@ -4554,8 +4545,8 @@
       <c r="E10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
       <c r="H10" s="1" t="s">
         <v>33</v>
       </c>
@@ -4565,25 +4556,25 @@
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
       <c r="A11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H11" s="2" t="s">
+      <c r="E11" s="3"/>
+      <c r="F11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>33</v>
       </c>
       <c r="I11" s="2" t="s">
@@ -4592,11 +4583,11 @@
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
       <c r="A12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>33</v>
@@ -4611,7 +4602,7 @@
         <v>33</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I12" s="2"/>
     </row>
@@ -4632,20 +4623,20 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="6" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="15.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="15.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="15.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="15.862142857142858" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="6" width="17.862142857142857" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="6" width="17.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="15.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="6" width="15.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="6" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="6" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="6" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="6" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="7" width="15.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="7" width="15.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="7" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="7" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="7" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="7" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -4654,8 +4645,8 @@
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -4673,8 +4664,8 @@
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -4692,8 +4683,8 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -4711,8 +4702,8 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -4730,8 +4721,8 @@
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -4749,8 +4740,8 @@
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -4768,8 +4759,8 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -4782,25 +4773,25 @@
       <c r="O7" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="4" t="s">
         <v>30</v>
       </c>
       <c r="H8" s="2"/>
@@ -4817,7 +4808,7 @@
         <v>31</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="8" t="s">
         <v>32</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -4826,12 +4817,10 @@
       <c r="E9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="8" t="s">
-        <v>34</v>
-      </c>
+      <c r="G9" s="1"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -4846,13 +4835,13 @@
         <v>26</v>
       </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="2"/>
+      <c r="C10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="3"/>
       <c r="F10" s="1" t="s">
         <v>33</v>
       </c>
@@ -4870,16 +4859,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
       <c r="A11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="2"/>
+      <c r="D11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="3"/>
       <c r="F11" s="1" t="s">
         <v>33</v>
       </c>
@@ -4896,15 +4885,15 @@
       <c r="O11" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
-      <c r="A12" s="3" t="s">
-        <v>38</v>
+      <c r="A12" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="2" t="s">
+      <c r="D12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>33</v>
       </c>
       <c r="F12" s="2" t="s">
@@ -4923,15 +4912,15 @@
       <c r="O12" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
-      <c r="A13" s="3" t="s">
-        <v>39</v>
+      <c r="A13" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="2" t="s">
+      <c r="D13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>33</v>
       </c>
       <c r="F13" s="2" t="s">
@@ -4950,15 +4939,15 @@
       <c r="O13" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="2" t="s">
+      <c r="D14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>33</v>
       </c>
       <c r="F14" s="2" t="s">
@@ -4977,15 +4966,15 @@
       <c r="O14" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
-      <c r="A15" s="3" t="s">
-        <v>40</v>
+      <c r="A15" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
-      <c r="D15" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="2" t="s">
+      <c r="D15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>33</v>
       </c>
       <c r="F15" s="2" t="s">
@@ -5004,8 +4993,8 @@
       <c r="O15" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25">
-      <c r="A16" s="3" t="s">
-        <v>41</v>
+      <c r="A16" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>

</xml_diff>

<commit_message>
ALE CH4 and CFC-113 data incorrectly added to data_combination for CMO
</commit_message>
<xml_diff>
--- a/data/agage/data_combination.xlsx
+++ b/data/agage/data_combination.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="CGO"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="92">
   <si>
     <t># File specifying when to use the various ALE/GAGE/AGAGE instruments</t>
   </si>
@@ -1971,7 +1971,7 @@
   </sheetPr>
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2269,7 +2269,7 @@
   </sheetPr>
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2429,8 +2429,12 @@
       <c r="A14" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D14" s="8" t="s">
         <v>69</v>
       </c>
@@ -2440,8 +2444,12 @@
       <c r="A15" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D15" s="8" t="s">
         <v>70</v>
       </c>

</xml_diff>

<commit_message>
Include ZEP ADS data for hcfc-124
</commit_message>
<xml_diff>
--- a/data/agage/data_combination.xlsx
+++ b/data/agage/data_combination.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joe Pitt\Downloads\240612\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JOEPIT~1\AppData\Local\Temp\scp16904\user\home\zh21490\agage-archive\data\agage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25BA94E1-AF54-434E-A510-0B1F93EF8DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A660818A-77D4-430A-89CB-470FF5EDA03E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CGO" sheetId="1" r:id="rId1"/>
@@ -383,7 +383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -404,9 +404,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="22" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1190,10 +1187,10 @@
       <c r="G19" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I19" s="9">
+      <c r="I19" s="8">
         <v>38481</v>
       </c>
-      <c r="J19" s="9">
+      <c r="J19" s="8">
         <v>38481</v>
       </c>
       <c r="L19" s="1" t="s">
@@ -1260,7 +1257,7 @@
       <c r="G21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H21" s="8" t="s">
+      <c r="H21" s="1" t="s">
         <v>33</v>
       </c>
       <c r="I21" s="1" t="s">
@@ -1601,8 +1598,8 @@
   </sheetPr>
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1725,13 +1722,12 @@
       <c r="A14" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B14" t="s">
-        <v>33</v>
-      </c>
       <c r="C14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
@@ -2242,7 +2238,7 @@
   </sheetPr>
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
@@ -2322,10 +2318,10 @@
       <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <v>39577.729166666664</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="8">
         <v>39577.729166666664</v>
       </c>
     </row>
@@ -2355,10 +2351,10 @@
       <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="8">
         <v>39675</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="8">
         <v>39675</v>
       </c>
     </row>
@@ -2465,10 +2461,10 @@
       <c r="A23" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="8">
         <v>39619</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23" s="8">
         <v>39619</v>
       </c>
     </row>
@@ -2789,10 +2785,10 @@
       <c r="E16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="8">
         <v>37940.625</v>
       </c>
-      <c r="H16" s="9">
+      <c r="H16" s="8">
         <v>37940.625</v>
       </c>
       <c r="J16" s="1" t="s">
@@ -2818,10 +2814,10 @@
       <c r="E17" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G17" s="8">
         <v>37940.625</v>
       </c>
-      <c r="H17" s="9">
+      <c r="H17" s="8">
         <v>37940.625</v>
       </c>
       <c r="J17" s="1" t="s">
@@ -2847,10 +2843,10 @@
       <c r="E18" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="8">
         <v>37940.625</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="8">
         <v>37940.625</v>
       </c>
       <c r="J18" s="1" t="s">
@@ -2876,10 +2872,10 @@
       <c r="E19" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="8">
         <v>38394.5</v>
       </c>
-      <c r="H19" s="9">
+      <c r="H19" s="8">
         <v>38394.5</v>
       </c>
       <c r="J19" s="1" t="s">
@@ -2905,10 +2901,10 @@
       <c r="E20" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="8">
         <v>37940.625</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20" s="8">
         <v>37940.625</v>
       </c>
       <c r="J20" s="1" t="s">
@@ -2934,10 +2930,10 @@
       <c r="E21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G21" s="9">
+      <c r="G21" s="8">
         <v>37940.625</v>
       </c>
-      <c r="H21" s="9">
+      <c r="H21" s="8">
         <v>37940.625</v>
       </c>
       <c r="J21" s="1" t="s">
@@ -2963,10 +2959,10 @@
       <c r="E22" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G22" s="9">
+      <c r="G22" s="8">
         <v>37940.625</v>
       </c>
-      <c r="H22" s="9">
+      <c r="H22" s="8">
         <v>37940.625</v>
       </c>
       <c r="J22" s="1" t="s">
@@ -2992,10 +2988,10 @@
       <c r="E23" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G23" s="9">
+      <c r="G23" s="8">
         <v>37940.625</v>
       </c>
-      <c r="H23" s="9">
+      <c r="H23" s="8">
         <v>37940.625</v>
       </c>
       <c r="J23" s="1" t="s">
@@ -3021,10 +3017,10 @@
       <c r="E24" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G24" s="9">
+      <c r="G24" s="8">
         <v>37940.625</v>
       </c>
-      <c r="H24" s="9">
+      <c r="H24" s="8">
         <v>37940.625</v>
       </c>
       <c r="J24" s="1" t="s">
@@ -3050,10 +3046,10 @@
       <c r="E25" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G25" s="9">
+      <c r="G25" s="8">
         <v>37940.625</v>
       </c>
-      <c r="H25" s="9">
+      <c r="H25" s="8">
         <v>37940.625</v>
       </c>
       <c r="J25" s="1" t="s">
@@ -3079,10 +3075,10 @@
       <c r="E26" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G26" s="9">
+      <c r="G26" s="8">
         <v>37940.625</v>
       </c>
-      <c r="H26" s="9">
+      <c r="H26" s="8">
         <v>37940.625</v>
       </c>
       <c r="J26" s="1" t="s">
@@ -3108,10 +3104,10 @@
       <c r="E27" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G27" s="9">
+      <c r="G27" s="8">
         <v>37940.625</v>
       </c>
-      <c r="H27" s="9">
+      <c r="H27" s="8">
         <v>37940.625</v>
       </c>
       <c r="J27" s="1" t="s">
@@ -3137,10 +3133,10 @@
       <c r="E28" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G28" s="9">
+      <c r="G28" s="8">
         <v>37940.625</v>
       </c>
-      <c r="H28" s="9">
+      <c r="H28" s="8">
         <v>37940.625</v>
       </c>
       <c r="J28" s="1" t="s">
@@ -3166,10 +3162,10 @@
       <c r="E29" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G29" s="9">
+      <c r="G29" s="8">
         <v>37940.625</v>
       </c>
-      <c r="H29" s="9">
+      <c r="H29" s="8">
         <v>37940.625</v>
       </c>
       <c r="J29" s="1" t="s">
@@ -3195,10 +3191,10 @@
       <c r="E30" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G30" s="9">
+      <c r="G30" s="8">
         <v>37940.625</v>
       </c>
-      <c r="H30" s="9">
+      <c r="H30" s="8">
         <v>37940.625</v>
       </c>
       <c r="J30" s="1" t="s">

</xml_diff>

<commit_message>
Include CGO ADS data for hcfc-124
</commit_message>
<xml_diff>
--- a/data/agage/data_combination.xlsx
+++ b/data/agage/data_combination.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JOEPIT~1\AppData\Local\Temp\scp16904\user\home\zh21490\agage-archive\data\agage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A660818A-77D4-430A-89CB-470FF5EDA03E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD1D418-0049-437B-8BB3-2A3B8FE589C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CGO" sheetId="1" r:id="rId1"/>
@@ -716,8 +716,8 @@
   </sheetPr>
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21:J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1257,13 +1257,13 @@
       <c r="G21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="H21" s="1"/>
       <c r="I21" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J21" s="1"/>
+        <v>90</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="L21" s="1" t="s">
         <v>33</v>
       </c>
@@ -1598,7 +1598,7 @@
   </sheetPr>
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
include TOB data in data_combination.xlsx
</commit_message>
<xml_diff>
--- a/data/agage/data_combination.xlsx
+++ b/data/agage/data_combination.xlsx
@@ -1,35 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JOEPIT~1\AppData\Local\Temp\scp16904\user\home\zh21490\agage-archive\data\agage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Python_Projects\agage-archive\data\agage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD1D418-0049-437B-8BB3-2A3B8FE589C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="13530" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="CGO" sheetId="1" r:id="rId1"/>
     <sheet name="CMN" sheetId="2" r:id="rId2"/>
     <sheet name="CMO" sheetId="3" r:id="rId3"/>
-    <sheet name="JFJ" sheetId="4" r:id="rId4"/>
-    <sheet name="MHD" sheetId="5" r:id="rId5"/>
+    <sheet name="MHD" sheetId="5" r:id="rId4"/>
+    <sheet name="JFJ" sheetId="4" r:id="rId5"/>
     <sheet name="RPB" sheetId="6" r:id="rId6"/>
     <sheet name="SMO" sheetId="7" r:id="rId7"/>
     <sheet name="TAC" sheetId="8" r:id="rId8"/>
     <sheet name="THD" sheetId="9" r:id="rId9"/>
     <sheet name="ZEP" sheetId="10" r:id="rId10"/>
+    <sheet name="TOB" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="139">
   <si>
     <t># File specifying when to use the various ALE/GAGE/AGAGE instruments</t>
   </si>
@@ -305,12 +305,153 @@
   </si>
   <si>
     <t>hcfc-124</t>
+  </si>
+  <si>
+    <t>SF6</t>
+  </si>
+  <si>
+    <t>SO2F2</t>
+  </si>
+  <si>
+    <t>HFO-1234yf</t>
+  </si>
+  <si>
+    <t>CH3Cl</t>
+  </si>
+  <si>
+    <t>CH3Br</t>
+  </si>
+  <si>
+    <t>CH3I</t>
+  </si>
+  <si>
+    <t>CH2Cl2</t>
+  </si>
+  <si>
+    <t>CHCl3</t>
+  </si>
+  <si>
+    <t>CH2Br2</t>
+  </si>
+  <si>
+    <t>CHBr3</t>
+  </si>
+  <si>
+    <t>TCE</t>
+  </si>
+  <si>
+    <t>PCE</t>
+  </si>
+  <si>
+    <t>ClCH2CH2Cl</t>
+  </si>
+  <si>
+    <t>ethyne</t>
+  </si>
+  <si>
+    <t>propane</t>
+  </si>
+  <si>
+    <t>c-propane</t>
+  </si>
+  <si>
+    <t>benzene</t>
+  </si>
+  <si>
+    <t>toluene</t>
+  </si>
+  <si>
+    <t>COS</t>
+  </si>
+  <si>
+    <t>taunus-tof start</t>
+  </si>
+  <si>
+    <t>taunus-tof end</t>
+  </si>
+  <si>
+    <t>taunus-ecd end</t>
+  </si>
+  <si>
+    <t>taunus-ecd start</t>
+  </si>
+  <si>
+    <t>2022-09-17 00:00</t>
+  </si>
+  <si>
+    <t>2020-10-12 00:00</t>
+  </si>
+  <si>
+    <t>2023-02-05 00:00</t>
+  </si>
+  <si>
+    <t>2018-05-18 00:00</t>
+  </si>
+  <si>
+    <t>PFC-218</t>
+  </si>
+  <si>
+    <t>PFC-318</t>
+  </si>
+  <si>
+    <t>HFC-32</t>
+  </si>
+  <si>
+    <t>HFC-125</t>
+  </si>
+  <si>
+    <t>HFC-134a</t>
+  </si>
+  <si>
+    <t>2024-05-01 00:00</t>
+  </si>
+  <si>
+    <t>HFC-143a</t>
+  </si>
+  <si>
+    <t>HFC-152a</t>
+  </si>
+  <si>
+    <t>HFC-236fa</t>
+  </si>
+  <si>
+    <t>HFC-245fa</t>
+  </si>
+  <si>
+    <t>HFC-365mfc</t>
+  </si>
+  <si>
+    <t>HFO-1234zeE</t>
+  </si>
+  <si>
+    <t>HCFO-1233ddE</t>
+  </si>
+  <si>
+    <t>2022-11-01 00:00</t>
+  </si>
+  <si>
+    <t>HCFC-22</t>
+  </si>
+  <si>
+    <t>HCFC-132b</t>
+  </si>
+  <si>
+    <t>HCFC-142b</t>
+  </si>
+  <si>
+    <t>HCFC-133a</t>
+  </si>
+  <si>
+    <t>CFC-115</t>
+  </si>
+  <si>
+    <t>H-1211</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -383,7 +524,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -409,9 +550,16 @@
     <xf numFmtId="22" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -710,17 +858,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I21" sqref="I21:J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
@@ -1592,7 +1740,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1602,7 +1750,7 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
@@ -1833,8 +1981,1051 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:I68"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>121</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>123</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="9"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>125</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="9"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>126</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>127</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="9"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>128</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="9"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>129</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="9"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="9"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>130</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="9"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>131</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="9"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>133</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="9"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>134</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H25" s="11"/>
+      <c r="I25" s="9"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>135</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="9"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>136</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="9"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>137</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="9"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>138</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="9"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="9"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="9"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>97</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="9"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="9"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="9"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>100</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="9"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="9"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>102</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="9"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>103</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="9"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>104</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="9"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>105</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="9"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>106</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="9"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>107</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="9"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>108</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G43" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H43" s="11"/>
+      <c r="I43" s="9"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>109</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F44" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G44" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H44" s="11"/>
+      <c r="I44" s="9"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>110</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E45" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="9"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="9"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="9"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B47" s="9"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="9"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B48" s="9"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="9"/>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B49" s="9"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="9"/>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B50" s="9"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="9"/>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B51" s="9"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="9"/>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B52" s="9"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="11"/>
+      <c r="G52" s="11"/>
+      <c r="H52" s="11"/>
+      <c r="I52" s="9"/>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B53" s="9"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
+      <c r="I53" s="9"/>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B54" s="9"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="11"/>
+      <c r="F54" s="11"/>
+      <c r="G54" s="11"/>
+      <c r="H54" s="11"/>
+      <c r="I54" s="9"/>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B55" s="9"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11"/>
+      <c r="I55" s="9"/>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B56" s="9"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="9"/>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B57" s="9"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="9"/>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B58" s="9"/>
+      <c r="C58" s="11"/>
+      <c r="D58" s="11"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
+      <c r="H58" s="11"/>
+      <c r="I58" s="9"/>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B59" s="9"/>
+      <c r="C59" s="11"/>
+      <c r="D59" s="11"/>
+      <c r="E59" s="11"/>
+      <c r="F59" s="11"/>
+      <c r="G59" s="11"/>
+      <c r="H59" s="11"/>
+      <c r="I59" s="9"/>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B60" s="9"/>
+      <c r="C60" s="11"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="11"/>
+      <c r="F60" s="11"/>
+      <c r="G60" s="11"/>
+      <c r="H60" s="11"/>
+      <c r="I60" s="9"/>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B61" s="9"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="11"/>
+      <c r="H61" s="11"/>
+      <c r="I61" s="9"/>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B62" s="9"/>
+      <c r="C62" s="11"/>
+      <c r="D62" s="11"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="11"/>
+      <c r="G62" s="11"/>
+      <c r="H62" s="11"/>
+      <c r="I62" s="9"/>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B63" s="9"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="11"/>
+      <c r="E63" s="11"/>
+      <c r="F63" s="11"/>
+      <c r="G63" s="11"/>
+      <c r="H63" s="11"/>
+      <c r="I63" s="9"/>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B64" s="9"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
+      <c r="G64" s="11"/>
+      <c r="H64" s="11"/>
+      <c r="I64" s="9"/>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B65" s="9"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="11"/>
+      <c r="E65" s="11"/>
+      <c r="F65" s="11"/>
+      <c r="G65" s="11"/>
+      <c r="H65" s="11"/>
+      <c r="I65" s="9"/>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B66" s="9"/>
+      <c r="C66" s="11"/>
+      <c r="D66" s="11"/>
+      <c r="E66" s="11"/>
+      <c r="F66" s="11"/>
+      <c r="G66" s="11"/>
+      <c r="H66" s="11"/>
+      <c r="I66" s="9"/>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B67" s="9"/>
+      <c r="C67" s="11"/>
+      <c r="D67" s="11"/>
+      <c r="E67" s="11"/>
+      <c r="F67" s="11"/>
+      <c r="G67" s="11"/>
+      <c r="H67" s="11"/>
+      <c r="I67" s="9"/>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B68" s="9"/>
+      <c r="C68" s="11"/>
+      <c r="D68" s="11"/>
+      <c r="E68" s="11"/>
+      <c r="F68" s="11"/>
+      <c r="G68" s="11"/>
+      <c r="H68" s="11"/>
+      <c r="I68" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1842,7 +3033,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
@@ -2074,7 +3265,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -2082,7 +3273,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
@@ -2232,249 +3423,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:E23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="8">
-        <v>39577.729166666664</v>
-      </c>
-      <c r="D10" s="8">
-        <v>39577.729166666664</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="8">
-        <v>39675</v>
-      </c>
-      <c r="D13" s="8">
-        <v>39675</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" s="8">
-        <v>39619</v>
-      </c>
-      <c r="D23" s="8">
-        <v>39619</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -2484,7 +3433,7 @@
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
@@ -3209,8 +4158,250 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:E23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="8">
+        <v>39577.729166666664</v>
+      </c>
+      <c r="D10" s="8">
+        <v>39577.729166666664</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="8">
+        <v>39675</v>
+      </c>
+      <c r="D13" s="8">
+        <v>39675</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="8">
+        <v>39619</v>
+      </c>
+      <c r="D23" s="8">
+        <v>39619</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -3218,7 +4409,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
@@ -3509,7 +4700,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -3517,7 +4708,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
@@ -3840,7 +5031,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -3848,7 +5039,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
@@ -4025,7 +5216,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -4033,7 +5224,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="15.85546875" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Tidied up data selection files for TOB and improved error checking slightly
</commit_message>
<xml_diff>
--- a/data/agage/data_combination.xlsx
+++ b/data/agage/data_combination.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Python_Projects\agage-archive\data\agage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/code/agage-archive/data/agage/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50E2FC7-921D-2E44-B77E-C878F118C274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="13530" activeTab="10"/>
+    <workbookView xWindow="10640" yWindow="500" windowWidth="36340" windowHeight="19760" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CGO" sheetId="1" r:id="rId1"/>
@@ -21,15 +22,28 @@
     <sheet name="SMO" sheetId="7" r:id="rId7"/>
     <sheet name="TAC" sheetId="8" r:id="rId8"/>
     <sheet name="THD" sheetId="9" r:id="rId9"/>
-    <sheet name="ZEP" sheetId="10" r:id="rId10"/>
-    <sheet name="TOB" sheetId="11" r:id="rId11"/>
+    <sheet name="TOB" sheetId="11" r:id="rId10"/>
+    <sheet name="ZEP" sheetId="10" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="125">
   <si>
     <t># File specifying when to use the various ALE/GAGE/AGAGE instruments</t>
   </si>
@@ -220,9 +234,6 @@
     <t>2010-12-01 00:00</t>
   </si>
   <si>
-    <t>pce</t>
-  </si>
-  <si>
     <t>2008-04-19 00:00</t>
   </si>
   <si>
@@ -307,69 +318,6 @@
     <t>hcfc-124</t>
   </si>
   <si>
-    <t>SF6</t>
-  </si>
-  <si>
-    <t>SO2F2</t>
-  </si>
-  <si>
-    <t>HFO-1234yf</t>
-  </si>
-  <si>
-    <t>CH3Cl</t>
-  </si>
-  <si>
-    <t>CH3Br</t>
-  </si>
-  <si>
-    <t>CH3I</t>
-  </si>
-  <si>
-    <t>CH2Cl2</t>
-  </si>
-  <si>
-    <t>CHCl3</t>
-  </si>
-  <si>
-    <t>CH2Br2</t>
-  </si>
-  <si>
-    <t>CHBr3</t>
-  </si>
-  <si>
-    <t>TCE</t>
-  </si>
-  <si>
-    <t>PCE</t>
-  </si>
-  <si>
-    <t>ClCH2CH2Cl</t>
-  </si>
-  <si>
-    <t>ethyne</t>
-  </si>
-  <si>
-    <t>propane</t>
-  </si>
-  <si>
-    <t>c-propane</t>
-  </si>
-  <si>
-    <t>benzene</t>
-  </si>
-  <si>
-    <t>toluene</t>
-  </si>
-  <si>
-    <t>COS</t>
-  </si>
-  <si>
-    <t>taunus-tof start</t>
-  </si>
-  <si>
-    <t>taunus-tof end</t>
-  </si>
-  <si>
     <t>taunus-ecd end</t>
   </si>
   <si>
@@ -388,70 +336,94 @@
     <t>2018-05-18 00:00</t>
   </si>
   <si>
-    <t>PFC-218</t>
-  </si>
-  <si>
-    <t>PFC-318</t>
-  </si>
-  <si>
-    <t>HFC-32</t>
-  </si>
-  <si>
-    <t>HFC-125</t>
-  </si>
-  <si>
-    <t>HFC-134a</t>
-  </si>
-  <si>
     <t>2024-05-01 00:00</t>
   </si>
   <si>
-    <t>HFC-143a</t>
-  </si>
-  <si>
-    <t>HFC-152a</t>
-  </si>
-  <si>
-    <t>HFC-236fa</t>
-  </si>
-  <si>
-    <t>HFC-245fa</t>
-  </si>
-  <si>
-    <t>HFC-365mfc</t>
-  </si>
-  <si>
-    <t>HFO-1234zeE</t>
-  </si>
-  <si>
-    <t>HCFO-1233ddE</t>
-  </si>
-  <si>
     <t>2022-11-01 00:00</t>
   </si>
   <si>
-    <t>HCFC-22</t>
-  </si>
-  <si>
-    <t>HCFC-132b</t>
-  </si>
-  <si>
-    <t>HCFC-142b</t>
-  </si>
-  <si>
-    <t>HCFC-133a</t>
-  </si>
-  <si>
-    <t>CFC-115</t>
-  </si>
-  <si>
-    <t>H-1211</t>
+    <t>GCTOFMS start</t>
+  </si>
+  <si>
+    <t>GCTOFMS end</t>
+  </si>
+  <si>
+    <t>c3f8</t>
+  </si>
+  <si>
+    <t>c4f8</t>
+  </si>
+  <si>
+    <t>so2f2</t>
+  </si>
+  <si>
+    <t>hfc-32</t>
+  </si>
+  <si>
+    <t>hfc-143a</t>
+  </si>
+  <si>
+    <t>hfc-236fa</t>
+  </si>
+  <si>
+    <t>hfo-1234yf</t>
+  </si>
+  <si>
+    <t>hfo-1234zee</t>
+  </si>
+  <si>
+    <t>hcfc-132b</t>
+  </si>
+  <si>
+    <t>hcfc-133a</t>
+  </si>
+  <si>
+    <t>cfc-115</t>
+  </si>
+  <si>
+    <t>ch3i</t>
+  </si>
+  <si>
+    <t>ch2br2</t>
+  </si>
+  <si>
+    <t>chbr3</t>
+  </si>
+  <si>
+    <t>clch2ch2cl</t>
+  </si>
+  <si>
+    <t>cos</t>
+  </si>
+  <si>
+    <t>c2h2</t>
+  </si>
+  <si>
+    <t>c3h8</t>
+  </si>
+  <si>
+    <t>c3h6</t>
+  </si>
+  <si>
+    <t>c6h6</t>
+  </si>
+  <si>
+    <t>c6h5ch3</t>
+  </si>
+  <si>
+    <t>ccl2ccl2</t>
+  </si>
+  <si>
+    <t>chclccl2</t>
+  </si>
+  <si>
+    <t>hcfo-1233zde</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -559,7 +531,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -572,6 +544,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -858,65 +834,65 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21:J21"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -957,7 +933,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
@@ -968,58 +944,58 @@
         <v>33</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="H9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="H10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="G10" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>89</v>
-      </c>
       <c r="L10" s="1" t="s">
         <v>33</v>
       </c>
@@ -1027,21 +1003,21 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>33</v>
@@ -1062,21 +1038,21 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>33</v>
@@ -1097,7 +1073,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
@@ -1108,13 +1084,13 @@
         <v>33</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>54</v>
@@ -1138,21 +1114,21 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>33</v>
@@ -1173,21 +1149,21 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>33</v>
@@ -1208,7 +1184,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -1231,10 +1207,10 @@
         <v>33</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>33</v>
@@ -1243,7 +1219,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -1266,10 +1242,10 @@
         <v>33</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>33</v>
@@ -1278,7 +1254,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -1301,10 +1277,10 @@
         <v>33</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>33</v>
@@ -1313,7 +1289,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -1348,7 +1324,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -1371,21 +1347,21 @@
         <v>33</v>
       </c>
       <c r="I20" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>33</v>
@@ -1407,10 +1383,10 @@
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>33</v>
@@ -1419,7 +1395,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
@@ -1442,10 +1418,10 @@
         <v>33</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>33</v>
@@ -1454,7 +1430,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
@@ -1477,10 +1453,10 @@
         <v>33</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>33</v>
@@ -1489,7 +1465,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
@@ -1512,10 +1488,10 @@
         <v>33</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>33</v>
@@ -1524,7 +1500,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
@@ -1547,10 +1523,10 @@
         <v>33</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>33</v>
@@ -1559,7 +1535,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>22</v>
       </c>
@@ -1582,10 +1558,10 @@
         <v>33</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>33</v>
@@ -1594,7 +1570,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>23</v>
       </c>
@@ -1617,10 +1593,10 @@
         <v>33</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>33</v>
@@ -1629,7 +1605,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>24</v>
       </c>
@@ -1652,10 +1628,10 @@
         <v>33</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>33</v>
@@ -1664,7 +1640,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
@@ -1687,10 +1663,10 @@
         <v>33</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>33</v>
@@ -1699,9 +1675,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>63</v>
+        <v>122</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>33</v>
@@ -1722,10 +1698,10 @@
         <v>33</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L30" s="1" t="s">
         <v>33</v>
@@ -1740,321 +1716,79 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:E23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView topLeftCell="A3" zoomScale="107" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:A38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>10</v>
@@ -2064,12 +1798,12 @@
       </c>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10" t="s">
@@ -2083,12 +1817,12 @@
       <c r="H9" s="10"/>
       <c r="I9" s="9"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11" t="s">
@@ -2102,9 +1836,9 @@
       <c r="H10" s="11"/>
       <c r="I10" s="9"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>92</v>
+        <v>44</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>33</v>
@@ -2113,22 +1847,22 @@
         <v>33</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
       <c r="I11" s="9"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11" t="s">
@@ -2142,12 +1876,12 @@
       <c r="H12" s="11"/>
       <c r="I12" s="9"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11" t="s">
@@ -2159,14 +1893,13 @@
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
-      <c r="I13" s="9"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>122</v>
+        <v>12</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11" t="s">
@@ -2178,11 +1911,10 @@
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
-      <c r="I14" s="9"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>123</v>
+        <v>14</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>33</v>
@@ -2197,18 +1929,17 @@
         <v>33</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
-      <c r="I15" s="9"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11" t="s">
@@ -2220,14 +1951,13 @@
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
-      <c r="I16" s="9"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>126</v>
+        <v>15</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11" t="s">
@@ -2239,14 +1969,13 @@
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
       <c r="H17" s="11"/>
-      <c r="I17" s="9"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11" t="s">
@@ -2258,14 +1987,13 @@
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
       <c r="H18" s="11"/>
-      <c r="I18" s="9"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>128</v>
+        <v>65</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="C19" s="11"/>
       <c r="D19" s="11" t="s">
@@ -2277,14 +2005,13 @@
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
-      <c r="I19" s="9"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>129</v>
+        <v>16</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11" t="s">
@@ -2296,14 +2023,13 @@
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
-      <c r="I20" s="9"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="11" t="s">
@@ -2315,14 +2041,13 @@
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
-      <c r="I21" s="9"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>130</v>
+        <v>108</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="11" t="s">
@@ -2334,14 +2059,13 @@
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
-      <c r="I22" s="9"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11" t="s">
@@ -2353,14 +2077,13 @@
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
-      <c r="I23" s="9"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>132</v>
+        <v>98</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11" t="s">
@@ -2372,11 +2095,10 @@
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
-      <c r="I24" s="9"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>33</v>
@@ -2397,14 +2119,13 @@
         <v>33</v>
       </c>
       <c r="H25" s="11"/>
-      <c r="I25" s="9"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>135</v>
+        <v>19</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="11" t="s">
@@ -2416,14 +2137,13 @@
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
       <c r="H26" s="11"/>
-      <c r="I26" s="9"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>136</v>
+        <v>110</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="11" t="s">
@@ -2435,14 +2155,13 @@
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
-      <c r="I27" s="9"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>137</v>
+        <v>111</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="C28" s="11"/>
       <c r="D28" s="11" t="s">
@@ -2454,14 +2173,13 @@
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
       <c r="H28" s="11"/>
-      <c r="I28" s="9"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>138</v>
+        <v>20</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="C29" s="11"/>
       <c r="D29" s="11" t="s">
@@ -2473,14 +2191,13 @@
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
       <c r="H29" s="11"/>
-      <c r="I29" s="9"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>95</v>
+        <v>22</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="11" t="s">
@@ -2492,14 +2209,13 @@
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
       <c r="H30" s="11"/>
-      <c r="I30" s="9"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="9" t="s">
         <v>96</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>118</v>
       </c>
       <c r="C31" s="11"/>
       <c r="D31" s="11" t="s">
@@ -2511,14 +2227,13 @@
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
       <c r="H31" s="11"/>
-      <c r="I31" s="9"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="11" t="s">
@@ -2530,14 +2245,13 @@
       <c r="F32" s="11"/>
       <c r="G32" s="11"/>
       <c r="H32" s="11"/>
-      <c r="I32" s="9"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C33" s="11"/>
       <c r="D33" s="11" t="s">
@@ -2549,14 +2263,13 @@
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
       <c r="H33" s="11"/>
-      <c r="I33" s="9"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>99</v>
+        <v>25</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="11" t="s">
@@ -2568,14 +2281,13 @@
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
       <c r="H34" s="11"/>
-      <c r="I34" s="9"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C35" s="11"/>
       <c r="D35" s="11" t="s">
@@ -2587,14 +2299,13 @@
       <c r="F35" s="11"/>
       <c r="G35" s="11"/>
       <c r="H35" s="11"/>
-      <c r="I35" s="9"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C36" s="11"/>
       <c r="D36" s="11" t="s">
@@ -2606,14 +2317,13 @@
       <c r="F36" s="11"/>
       <c r="G36" s="11"/>
       <c r="H36" s="11"/>
-      <c r="I36" s="9"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>102</v>
+        <v>123</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C37" s="11"/>
       <c r="D37" s="11" t="s">
@@ -2625,14 +2335,13 @@
       <c r="F37" s="11"/>
       <c r="G37" s="11"/>
       <c r="H37" s="11"/>
-      <c r="I37" s="9"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>103</v>
+        <v>122</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="11" t="s">
@@ -2644,14 +2353,13 @@
       <c r="F38" s="11"/>
       <c r="G38" s="11"/>
       <c r="H38" s="11"/>
-      <c r="I38" s="9"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="11" t="s">
@@ -2663,14 +2371,13 @@
       <c r="F39" s="11"/>
       <c r="G39" s="11"/>
       <c r="H39" s="11"/>
-      <c r="I39" s="9"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C40" s="11"/>
       <c r="D40" s="11" t="s">
@@ -2682,14 +2389,13 @@
       <c r="F40" s="11"/>
       <c r="G40" s="11"/>
       <c r="H40" s="11"/>
-      <c r="I40" s="9"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C41" s="11"/>
       <c r="D41" s="11" t="s">
@@ -2701,14 +2407,13 @@
       <c r="F41" s="11"/>
       <c r="G41" s="11"/>
       <c r="H41" s="11"/>
-      <c r="I41" s="9"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C42" s="11"/>
       <c r="D42" s="11" t="s">
@@ -2720,14 +2425,13 @@
       <c r="F42" s="11"/>
       <c r="G42" s="11"/>
       <c r="H42" s="11"/>
-      <c r="I42" s="9"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C43" s="11"/>
       <c r="D43" s="11" t="s">
@@ -2743,11 +2447,10 @@
         <v>33</v>
       </c>
       <c r="H43" s="11"/>
-      <c r="I43" s="9"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="B44" s="9" t="s">
         <v>33</v>
@@ -2768,14 +2471,13 @@
         <v>33</v>
       </c>
       <c r="H44" s="11"/>
-      <c r="I44" s="9"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C45" s="11"/>
       <c r="D45" s="11" t="s">
@@ -2787,9 +2489,8 @@
       <c r="F45" s="11"/>
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
-      <c r="I45" s="9"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B46" s="9"/>
       <c r="C46" s="11"/>
       <c r="D46" s="11"/>
@@ -2799,7 +2500,7 @@
       <c r="H46" s="11"/>
       <c r="I46" s="9"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B47" s="9"/>
       <c r="C47" s="11"/>
       <c r="D47" s="11"/>
@@ -2809,7 +2510,7 @@
       <c r="H47" s="11"/>
       <c r="I47" s="9"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B48" s="9"/>
       <c r="C48" s="11"/>
       <c r="D48" s="11"/>
@@ -2819,7 +2520,7 @@
       <c r="H48" s="11"/>
       <c r="I48" s="9"/>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B49" s="9"/>
       <c r="C49" s="11"/>
       <c r="D49" s="11"/>
@@ -2829,7 +2530,7 @@
       <c r="H49" s="11"/>
       <c r="I49" s="9"/>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B50" s="9"/>
       <c r="C50" s="11"/>
       <c r="D50" s="11"/>
@@ -2839,7 +2540,7 @@
       <c r="H50" s="11"/>
       <c r="I50" s="9"/>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B51" s="9"/>
       <c r="C51" s="11"/>
       <c r="D51" s="11"/>
@@ -2849,7 +2550,7 @@
       <c r="H51" s="11"/>
       <c r="I51" s="9"/>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B52" s="9"/>
       <c r="C52" s="11"/>
       <c r="D52" s="11"/>
@@ -2859,7 +2560,7 @@
       <c r="H52" s="11"/>
       <c r="I52" s="9"/>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B53" s="9"/>
       <c r="C53" s="11"/>
       <c r="D53" s="11"/>
@@ -2869,7 +2570,7 @@
       <c r="H53" s="11"/>
       <c r="I53" s="9"/>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B54" s="9"/>
       <c r="C54" s="11"/>
       <c r="D54" s="11"/>
@@ -2879,7 +2580,7 @@
       <c r="H54" s="11"/>
       <c r="I54" s="9"/>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B55" s="9"/>
       <c r="C55" s="11"/>
       <c r="D55" s="11"/>
@@ -2889,7 +2590,7 @@
       <c r="H55" s="11"/>
       <c r="I55" s="9"/>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B56" s="9"/>
       <c r="C56" s="11"/>
       <c r="D56" s="11"/>
@@ -2899,7 +2600,7 @@
       <c r="H56" s="11"/>
       <c r="I56" s="9"/>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B57" s="9"/>
       <c r="C57" s="11"/>
       <c r="D57" s="11"/>
@@ -2909,7 +2610,7 @@
       <c r="H57" s="11"/>
       <c r="I57" s="9"/>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B58" s="9"/>
       <c r="C58" s="11"/>
       <c r="D58" s="11"/>
@@ -2919,7 +2620,7 @@
       <c r="H58" s="11"/>
       <c r="I58" s="9"/>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B59" s="9"/>
       <c r="C59" s="11"/>
       <c r="D59" s="11"/>
@@ -2929,7 +2630,7 @@
       <c r="H59" s="11"/>
       <c r="I59" s="9"/>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B60" s="9"/>
       <c r="C60" s="11"/>
       <c r="D60" s="11"/>
@@ -2939,7 +2640,7 @@
       <c r="H60" s="11"/>
       <c r="I60" s="9"/>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B61" s="9"/>
       <c r="C61" s="11"/>
       <c r="D61" s="11"/>
@@ -2949,7 +2650,7 @@
       <c r="H61" s="11"/>
       <c r="I61" s="9"/>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B62" s="9"/>
       <c r="C62" s="11"/>
       <c r="D62" s="11"/>
@@ -2959,7 +2660,7 @@
       <c r="H62" s="11"/>
       <c r="I62" s="9"/>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B63" s="9"/>
       <c r="C63" s="11"/>
       <c r="D63" s="11"/>
@@ -2969,7 +2670,7 @@
       <c r="H63" s="11"/>
       <c r="I63" s="9"/>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B64" s="9"/>
       <c r="C64" s="11"/>
       <c r="D64" s="11"/>
@@ -2979,7 +2680,7 @@
       <c r="H64" s="11"/>
       <c r="I64" s="9"/>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B65" s="9"/>
       <c r="C65" s="11"/>
       <c r="D65" s="11"/>
@@ -2989,7 +2690,7 @@
       <c r="H65" s="11"/>
       <c r="I65" s="9"/>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B66" s="9"/>
       <c r="C66" s="11"/>
       <c r="D66" s="11"/>
@@ -2999,7 +2700,7 @@
       <c r="H66" s="11"/>
       <c r="I66" s="9"/>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B67" s="9"/>
       <c r="C67" s="11"/>
       <c r="D67" s="11"/>
@@ -3009,7 +2710,7 @@
       <c r="H67" s="11"/>
       <c r="I67" s="9"/>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B68" s="9"/>
       <c r="C68" s="11"/>
       <c r="D68" s="11"/>
@@ -3024,68 +2725,70 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>70</v>
+        <v>8</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>71</v>
+        <v>9</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>10</v>
@@ -3094,169 +2797,411 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:E23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>63</v>
+        <v>122</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -3265,7 +3210,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -3273,51 +3218,51 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -3334,62 +3279,62 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>38</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>37</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>40</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>31</v>
       </c>
@@ -3400,10 +3345,10 @@
         <v>33</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>35</v>
       </c>
@@ -3414,7 +3359,7 @@
         <v>33</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -3423,64 +3368,64 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -3515,7 +3460,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>38</v>
       </c>
@@ -3544,7 +3489,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>37</v>
       </c>
@@ -3573,7 +3518,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>35</v>
       </c>
@@ -3602,7 +3547,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>26</v>
       </c>
@@ -3631,7 +3576,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>39</v>
       </c>
@@ -3660,7 +3605,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>40</v>
       </c>
@@ -3689,7 +3634,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>31</v>
       </c>
@@ -3718,7 +3663,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -3747,7 +3692,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -3776,7 +3721,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -3805,7 +3750,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -3834,7 +3779,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -3863,9 +3808,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>33</v>
@@ -3892,7 +3837,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
@@ -3921,7 +3866,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
@@ -3950,7 +3895,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
@@ -3979,7 +3924,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
@@ -4008,7 +3953,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>22</v>
       </c>
@@ -4037,7 +3982,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>23</v>
       </c>
@@ -4066,7 +4011,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>24</v>
       </c>
@@ -4095,7 +4040,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
@@ -4124,9 +4069,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>63</v>
+        <v>122</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>33</v>
@@ -4159,61 +4104,61 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -4230,18 +4175,18 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
@@ -4252,29 +4197,29 @@
         <v>39577.729166666664</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
@@ -4285,108 +4230,108 @@
         <v>39675</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="C22" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="D22" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>66</v>
       </c>
       <c r="C23" s="8">
         <v>39619</v>
@@ -4401,7 +4346,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -4409,54 +4354,54 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -4491,7 +4436,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>38</v>
       </c>
@@ -4520,7 +4465,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>37</v>
       </c>
@@ -4549,7 +4494,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>35</v>
       </c>
@@ -4578,7 +4523,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>26</v>
       </c>
@@ -4607,7 +4552,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>39</v>
       </c>
@@ -4636,7 +4581,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>40</v>
       </c>
@@ -4665,7 +4610,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>31</v>
       </c>
@@ -4700,7 +4645,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -4708,54 +4653,54 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -4790,7 +4735,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>38</v>
       </c>
@@ -4819,7 +4764,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>37</v>
       </c>
@@ -4848,7 +4793,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>35</v>
       </c>
@@ -4877,7 +4822,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>26</v>
       </c>
@@ -4906,7 +4851,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>39</v>
       </c>
@@ -4935,7 +4880,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>40</v>
       </c>
@@ -4964,7 +4909,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>31</v>
       </c>
@@ -4993,7 +4938,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -5031,62 +4976,64 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -5115,7 +5062,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>40</v>
       </c>
@@ -5138,7 +5085,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
@@ -5161,7 +5108,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>44</v>
       </c>
@@ -5187,7 +5134,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>46</v>
       </c>
@@ -5216,7 +5163,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -5224,54 +5171,54 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -5294,7 +5241,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
@@ -5312,7 +5259,7 @@
       </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -5330,7 +5277,7 @@
       </c>
       <c r="O10" s="6"/>
     </row>
-    <row r="11" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>35</v>
       </c>
@@ -5348,7 +5295,7 @@
       </c>
       <c r="O11" s="6"/>
     </row>
-    <row r="12" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>37</v>
       </c>
@@ -5365,7 +5312,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>38</v>
       </c>
@@ -5382,7 +5329,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
@@ -5399,7 +5346,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>39</v>
       </c>
@@ -5416,7 +5363,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
Updated to include Paul Krummel's instrument changes
</commit_message>
<xml_diff>
--- a/data/agage/data_combination.xlsx
+++ b/data/agage/data_combination.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/code/agage-archive/data/agage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50E2FC7-921D-2E44-B77E-C878F118C274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45AE9E8A-00B3-FB4B-A662-732C42F67B43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10640" yWindow="500" windowWidth="36340" windowHeight="19760" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2060" yWindow="500" windowWidth="36340" windowHeight="19760" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CGO" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="140">
   <si>
     <t># File specifying when to use the various ALE/GAGE/AGAGE instruments</t>
   </si>
@@ -300,15 +300,6 @@
     <t>2023-12-20 00:59</t>
   </si>
   <si>
-    <t>1994-01-01 00:00</t>
-  </si>
-  <si>
-    <t>2013-01-01 00:00</t>
-  </si>
-  <si>
-    <t>1994-03-15 00:00</t>
-  </si>
-  <si>
     <t>2010-06-01 00:00</t>
   </si>
   <si>
@@ -318,12 +309,6 @@
     <t>hcfc-124</t>
   </si>
   <si>
-    <t>taunus-ecd end</t>
-  </si>
-  <si>
-    <t>taunus-ecd start</t>
-  </si>
-  <si>
     <t>2022-09-17 00:00</t>
   </si>
   <si>
@@ -418,6 +403,66 @@
   </si>
   <si>
     <t>hcfo-1233zde</t>
+  </si>
+  <si>
+    <t>1993-08-12 06:30</t>
+  </si>
+  <si>
+    <t>2012-07-20 03:20</t>
+  </si>
+  <si>
+    <t>1982-03-31 16:00</t>
+  </si>
+  <si>
+    <t>1994-03-15 11:20</t>
+  </si>
+  <si>
+    <t>1993-08-10 13:00</t>
+  </si>
+  <si>
+    <t>1982-10-10 23:20</t>
+  </si>
+  <si>
+    <t>1993-08-10 05:00</t>
+  </si>
+  <si>
+    <t>1982-10-07 06:00</t>
+  </si>
+  <si>
+    <t>1993-09-15 22:50</t>
+  </si>
+  <si>
+    <t>1982-03-08 22:30</t>
+  </si>
+  <si>
+    <t>1993-08-14 05:00</t>
+  </si>
+  <si>
+    <t>2004-01-22 03:00</t>
+  </si>
+  <si>
+    <t>2005-02-11 01:00</t>
+  </si>
+  <si>
+    <t>GCECD start</t>
+  </si>
+  <si>
+    <t>GCECD end</t>
+  </si>
+  <si>
+    <t>GCPDD start</t>
+  </si>
+  <si>
+    <t>GCPDD end</t>
+  </si>
+  <si>
+    <t>h2</t>
+  </si>
+  <si>
+    <t>2005-07-19 04:00</t>
+  </si>
+  <si>
+    <t>2015-04-24 01:30</t>
   </si>
 </sst>
 </file>
@@ -496,7 +541,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -529,6 +574,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,10 +592,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -838,10 +882,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -849,50 +893,51 @@
     <col min="1" max="2" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="15.83203125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -915,25 +960,37 @@
         <v>28</v>
       </c>
       <c r="H8" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="L8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="M8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="N8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="O8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="P8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="Q8" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
@@ -943,58 +1000,73 @@
       <c r="C9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K9" s="1" t="s">
+      <c r="E9" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" s="10" t="s">
         <v>33</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P9" s="10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>87</v>
+      <c r="C10" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>123</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>33</v>
@@ -1002,33 +1074,42 @@
       <c r="M10" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N10" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K11" s="1" t="s">
+      <c r="C11" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K11" s="10" t="s">
         <v>33</v>
       </c>
       <c r="L11" s="1" t="s">
@@ -1037,33 +1118,45 @@
       <c r="M11" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K12" s="1" t="s">
+      <c r="C12" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K12" s="10" t="s">
         <v>33</v>
       </c>
       <c r="L12" s="1" t="s">
@@ -1072,8 +1165,20 @@
       <c r="M12" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
@@ -1083,63 +1188,73 @@
       <c r="C13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>87</v>
+      <c r="D13" s="1"/>
+      <c r="E13" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>124</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J13" s="5" t="s">
+      <c r="H13" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N13" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="K13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K14" s="1" t="s">
+      <c r="C14" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K14" s="10" t="s">
         <v>33</v>
       </c>
       <c r="L14" s="1" t="s">
@@ -1148,33 +1263,45 @@
       <c r="M14" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K15" s="1" t="s">
+      <c r="C15" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K15" s="10" t="s">
         <v>33</v>
       </c>
       <c r="L15" s="1" t="s">
@@ -1183,8 +1310,20 @@
       <c r="M15" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -1206,20 +1345,32 @@
       <c r="G16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="L16" s="1" t="s">
+      <c r="H16" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K16" s="10" t="s">
         <v>33</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -1241,20 +1392,32 @@
       <c r="G17" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I17" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H17" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M17" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="N17" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -1276,20 +1439,32 @@
       <c r="G18" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H18" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K18" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M18" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="N18" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -1311,20 +1486,32 @@
       <c r="G19" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I19" s="8">
-        <v>38481</v>
-      </c>
-      <c r="J19" s="8">
-        <v>38481</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H19" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J19" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K19" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M19" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="N19" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -1346,22 +1533,34 @@
       <c r="G20" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I20" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="L20" s="1" t="s">
+      <c r="H20" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K20" s="10" t="s">
         <v>33</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>33</v>
@@ -1381,21 +1580,33 @@
       <c r="G21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H21" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I21" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J21" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K21" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="L21" s="1"/>
+      <c r="M21" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="N21" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
@@ -1417,20 +1628,32 @@
       <c r="G22" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I22" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H22" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J22" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K22" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M22" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="N22" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
@@ -1452,20 +1675,32 @@
       <c r="G23" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I23" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H23" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J23" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K23" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M23" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="N23" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q23" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
@@ -1487,20 +1722,32 @@
       <c r="G24" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I24" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="L24" s="1" t="s">
+      <c r="H24" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J24" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K24" s="10" t="s">
         <v>33</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
@@ -1522,20 +1769,32 @@
       <c r="G25" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I25" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H25" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I25" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J25" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K25" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M25" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="N25" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>22</v>
       </c>
@@ -1557,20 +1816,32 @@
       <c r="G26" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I26" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H26" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J26" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K26" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M26" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="N26" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>23</v>
       </c>
@@ -1592,20 +1863,32 @@
       <c r="G27" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I27" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="L27" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M27" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H27" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I27" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J27" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K27" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M27" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="N27" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>24</v>
       </c>
@@ -1627,20 +1910,32 @@
       <c r="G28" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I28" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H28" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I28" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J28" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K28" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M28" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="N28" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
@@ -1656,28 +1951,42 @@
       <c r="E29" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>89</v>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J29" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K29" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="M29" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M29" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N29" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>33</v>
@@ -1697,16 +2006,123 @@
       <c r="G30" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I30" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="L30" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M30" s="1" t="s">
+      <c r="H30" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I30" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J30" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K30" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M30" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="N30" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q30" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I31" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N31" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="P31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q31" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J32" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="K32"/>
+      <c r="L32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N32" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O32" t="s">
+        <v>33</v>
+      </c>
+      <c r="P32" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q32" s="2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1722,8 +2138,8 @@
   </sheetPr>
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="107" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:A38"/>
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1779,16 +2195,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>92</v>
+        <v>133</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>91</v>
+        <v>134</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>10</v>
@@ -1800,10 +2216,10 @@
     </row>
     <row r="9" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10" t="s">
@@ -1819,10 +2235,10 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11" t="s">
@@ -1847,10 +2263,10 @@
         <v>33</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
@@ -1859,10 +2275,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11" t="s">
@@ -1878,10 +2294,10 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11" t="s">
@@ -1899,7 +2315,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11" t="s">
@@ -1929,17 +2345,17 @@
         <v>33</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11" t="s">
@@ -1957,7 +2373,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11" t="s">
@@ -1972,10 +2388,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11" t="s">
@@ -1993,7 +2409,7 @@
         <v>65</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C19" s="11"/>
       <c r="D19" s="11" t="s">
@@ -2011,7 +2427,7 @@
         <v>16</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11" t="s">
@@ -2026,10 +2442,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="11" t="s">
@@ -2044,10 +2460,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="11" t="s">
@@ -2062,10 +2478,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11" t="s">
@@ -2083,7 +2499,7 @@
         <v>17</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11" t="s">
@@ -2098,7 +2514,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>33</v>
@@ -2125,7 +2541,7 @@
         <v>19</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="11" t="s">
@@ -2140,10 +2556,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="11" t="s">
@@ -2158,10 +2574,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C28" s="11"/>
       <c r="D28" s="11" t="s">
@@ -2179,7 +2595,7 @@
         <v>20</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C29" s="11"/>
       <c r="D29" s="11" t="s">
@@ -2197,7 +2613,7 @@
         <v>22</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="11" t="s">
@@ -2215,7 +2631,7 @@
         <v>23</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C31" s="11"/>
       <c r="D31" s="11" t="s">
@@ -2230,10 +2646,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="11" t="s">
@@ -2251,7 +2667,7 @@
         <v>24</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C33" s="11"/>
       <c r="D33" s="11" t="s">
@@ -2269,7 +2685,7 @@
         <v>25</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="11" t="s">
@@ -2284,10 +2700,10 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C35" s="11"/>
       <c r="D35" s="11" t="s">
@@ -2302,10 +2718,10 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C36" s="11"/>
       <c r="D36" s="11" t="s">
@@ -2320,10 +2736,10 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C37" s="11"/>
       <c r="D37" s="11" t="s">
@@ -2338,10 +2754,10 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="11" t="s">
@@ -2356,10 +2772,10 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="11" t="s">
@@ -2374,10 +2790,10 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C40" s="11"/>
       <c r="D40" s="11" t="s">
@@ -2392,10 +2808,10 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C41" s="11"/>
       <c r="D41" s="11" t="s">
@@ -2410,10 +2826,10 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C42" s="11"/>
       <c r="D42" s="11" t="s">
@@ -2428,10 +2844,10 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C43" s="11"/>
       <c r="D43" s="11" t="s">
@@ -2450,7 +2866,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B44" s="9" t="s">
         <v>33</v>
@@ -2474,10 +2890,10 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C45" s="11"/>
       <c r="D45" s="11" t="s">
@@ -2732,7 +3148,7 @@
   </sheetPr>
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -2854,7 +3270,7 @@
     </row>
     <row r="14" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
@@ -2975,7 +3391,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3195,7 +3611,7 @@
     </row>
     <row r="23" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>84</v>
@@ -3375,7 +3791,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3810,7 +4226,7 @@
     </row>
     <row r="21" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>33</v>
@@ -4050,17 +4466,19 @@
       <c r="C29" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G29" s="8">
-        <v>37940.625</v>
-      </c>
-      <c r="H29" s="8">
-        <v>37940.625</v>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I29" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>33</v>
@@ -4071,7 +4489,7 @@
     </row>
     <row r="30" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>33</v>
@@ -4309,7 +4727,7 @@
     </row>
     <row r="21" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>63</v>
@@ -4352,7 +4770,9 @@
   </sheetPr>
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4651,7 +5071,9 @@
   </sheetPr>
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4960,9 +5382,7 @@
       <c r="H16" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="I16" s="1"/>
       <c r="J16" s="1" t="s">
         <v>33</v>
       </c>
@@ -5169,7 +5589,9 @@
   </sheetPr>
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Error in run script was missing several files. Fixed here
</commit_message>
<xml_diff>
--- a/data/agage/data_combination.xlsx
+++ b/data/agage/data_combination.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/code/agage-archive/data/agage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45AE9E8A-00B3-FB4B-A662-732C42F67B43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2621D0-9261-4C4E-9502-C0C39AF51D5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2060" yWindow="500" windowWidth="36340" windowHeight="19760" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2060" yWindow="500" windowWidth="36340" windowHeight="19760" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CGO" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="139">
   <si>
     <t># File specifying when to use the various ALE/GAGE/AGAGE instruments</t>
   </si>
@@ -178,9 +178,6 @@
   </si>
   <si>
     <t>sf6</t>
-  </si>
-  <si>
-    <t>2018-03-14 00:00</t>
   </si>
   <si>
     <t>co</t>
@@ -541,7 +538,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -572,9 +569,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -885,7 +879,7 @@
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -942,16 +936,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>27</v>
@@ -960,16 +954,16 @@
         <v>28</v>
       </c>
       <c r="H8" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="J8" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="K8" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>136</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>8</v>
@@ -1001,40 +995,40 @@
         <v>33</v>
       </c>
       <c r="E9" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="G9" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="H9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P9" s="10" t="s">
         <v>120</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="K9" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="P9" s="10" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1042,19 +1036,19 @@
         <v>26</v>
       </c>
       <c r="C10" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="F10" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="E10" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>123</v>
-      </c>
       <c r="G10" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H10" s="10" t="s">
         <v>33</v>
@@ -1075,7 +1069,7 @@
         <v>33</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>33</v>
@@ -1089,16 +1083,16 @@
         <v>38</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H11" s="10" t="s">
         <v>33</v>
@@ -1136,16 +1130,16 @@
         <v>37</v>
       </c>
       <c r="C12" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="F12" s="10" t="s">
         <v>125</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>126</v>
       </c>
       <c r="H12" s="10" t="s">
         <v>33</v>
@@ -1190,13 +1184,13 @@
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H13" s="10" t="s">
         <v>33</v>
@@ -1217,7 +1211,7 @@
         <v>33</v>
       </c>
       <c r="N13" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>33</v>
@@ -1234,16 +1228,16 @@
         <v>39</v>
       </c>
       <c r="C14" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="E14" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="F14" s="10" t="s">
         <v>127</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>128</v>
       </c>
       <c r="H14" s="10" t="s">
         <v>33</v>
@@ -1281,16 +1275,16 @@
         <v>40</v>
       </c>
       <c r="C15" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E15" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="F15" s="10" t="s">
         <v>129</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>130</v>
       </c>
       <c r="H15" s="10" t="s">
         <v>33</v>
@@ -1358,10 +1352,10 @@
         <v>33</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P16" s="1" t="s">
         <v>33</v>
@@ -1405,10 +1399,10 @@
         <v>33</v>
       </c>
       <c r="M17" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N17" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="P17" s="1" t="s">
         <v>33</v>
@@ -1452,10 +1446,10 @@
         <v>33</v>
       </c>
       <c r="M18" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N18" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="P18" s="1" t="s">
         <v>33</v>
@@ -1499,10 +1493,10 @@
         <v>33</v>
       </c>
       <c r="M19" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N19" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="P19" s="1" t="s">
         <v>33</v>
@@ -1546,10 +1540,10 @@
         <v>33</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P20" s="1" t="s">
         <v>33</v>
@@ -1560,7 +1554,7 @@
     </row>
     <row r="21" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>33</v>
@@ -1594,10 +1588,10 @@
       </c>
       <c r="L21" s="1"/>
       <c r="M21" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N21" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="P21" s="1" t="s">
         <v>33</v>
@@ -1641,10 +1635,10 @@
         <v>33</v>
       </c>
       <c r="M22" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N22" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="P22" s="1" t="s">
         <v>33</v>
@@ -1688,10 +1682,10 @@
         <v>33</v>
       </c>
       <c r="M23" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N23" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="P23" s="1" t="s">
         <v>33</v>
@@ -1735,10 +1729,10 @@
         <v>33</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P24" s="1" t="s">
         <v>33</v>
@@ -1782,10 +1776,10 @@
         <v>33</v>
       </c>
       <c r="M25" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N25" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="P25" s="1" t="s">
         <v>33</v>
@@ -1829,10 +1823,10 @@
         <v>33</v>
       </c>
       <c r="M26" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N26" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="P26" s="1" t="s">
         <v>33</v>
@@ -1876,10 +1870,10 @@
         <v>33</v>
       </c>
       <c r="M27" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N27" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="P27" s="1" t="s">
         <v>33</v>
@@ -1923,10 +1917,10 @@
         <v>33</v>
       </c>
       <c r="M28" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N28" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="P28" s="1" t="s">
         <v>33</v>
@@ -1986,7 +1980,7 @@
     </row>
     <row r="30" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>33</v>
@@ -2019,10 +2013,10 @@
         <v>33</v>
       </c>
       <c r="M30" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N30" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="P30" s="1" t="s">
         <v>33</v>
@@ -2054,7 +2048,7 @@
         <v>33</v>
       </c>
       <c r="I31" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J31" s="2" t="s">
         <v>33</v>
@@ -2069,7 +2063,7 @@
         <v>33</v>
       </c>
       <c r="N31" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P31" s="2" t="s">
         <v>33</v>
@@ -2080,7 +2074,7 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>33</v>
@@ -2095,7 +2089,7 @@
         <v>33</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>33</v>
@@ -2104,7 +2098,7 @@
         <v>33</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K32"/>
       <c r="L32" t="s">
@@ -2138,7 +2132,7 @@
   </sheetPr>
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="107" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -2195,16 +2189,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>95</v>
-      </c>
       <c r="D8" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>133</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>10</v>
@@ -2216,10 +2210,10 @@
     </row>
     <row r="9" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10" t="s">
@@ -2235,10 +2229,10 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11" t="s">
@@ -2263,10 +2257,10 @@
         <v>33</v>
       </c>
       <c r="D11" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="E11" s="11" t="s">
         <v>89</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>90</v>
       </c>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
@@ -2275,10 +2269,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11" t="s">
@@ -2294,10 +2288,10 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11" t="s">
@@ -2315,7 +2309,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11" t="s">
@@ -2345,17 +2339,17 @@
         <v>33</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11" t="s">
@@ -2373,7 +2367,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11" t="s">
@@ -2388,10 +2382,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11" t="s">
@@ -2406,10 +2400,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C19" s="11"/>
       <c r="D19" s="11" t="s">
@@ -2427,7 +2421,7 @@
         <v>16</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11" t="s">
@@ -2442,10 +2436,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="11" t="s">
@@ -2460,10 +2454,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="11" t="s">
@@ -2478,10 +2472,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11" t="s">
@@ -2499,7 +2493,7 @@
         <v>17</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11" t="s">
@@ -2514,7 +2508,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>33</v>
@@ -2541,7 +2535,7 @@
         <v>19</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="11" t="s">
@@ -2556,10 +2550,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="11" t="s">
@@ -2574,10 +2568,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C28" s="11"/>
       <c r="D28" s="11" t="s">
@@ -2595,7 +2589,7 @@
         <v>20</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C29" s="11"/>
       <c r="D29" s="11" t="s">
@@ -2613,7 +2607,7 @@
         <v>22</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="11" t="s">
@@ -2631,7 +2625,7 @@
         <v>23</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C31" s="11"/>
       <c r="D31" s="11" t="s">
@@ -2646,10 +2640,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="11" t="s">
@@ -2667,7 +2661,7 @@
         <v>24</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C33" s="11"/>
       <c r="D33" s="11" t="s">
@@ -2685,7 +2679,7 @@
         <v>25</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="11" t="s">
@@ -2700,10 +2694,10 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C35" s="11"/>
       <c r="D35" s="11" t="s">
@@ -2718,10 +2712,10 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C36" s="11"/>
       <c r="D36" s="11" t="s">
@@ -2736,10 +2730,10 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C37" s="11"/>
       <c r="D37" s="11" t="s">
@@ -2754,10 +2748,10 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="11" t="s">
@@ -2772,10 +2766,10 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="11" t="s">
@@ -2790,10 +2784,10 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C40" s="11"/>
       <c r="D40" s="11" t="s">
@@ -2808,10 +2802,10 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C41" s="11"/>
       <c r="D41" s="11" t="s">
@@ -2826,10 +2820,10 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C42" s="11"/>
       <c r="D42" s="11" t="s">
@@ -2844,10 +2838,10 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C43" s="11"/>
       <c r="D43" s="11" t="s">
@@ -2866,7 +2860,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B44" s="9" t="s">
         <v>33</v>
@@ -2890,10 +2884,10 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C45" s="11"/>
       <c r="D45" s="11" t="s">
@@ -3270,7 +3264,7 @@
     </row>
     <row r="14" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
@@ -3443,10 +3437,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>10</v>
@@ -3460,10 +3454,10 @@
         <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3471,10 +3465,10 @@
         <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3482,10 +3476,10 @@
         <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3493,10 +3487,10 @@
         <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3504,10 +3498,10 @@
         <v>17</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3515,10 +3509,10 @@
         <v>18</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3526,10 +3520,10 @@
         <v>19</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3537,10 +3531,10 @@
         <v>20</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3548,10 +3542,10 @@
         <v>21</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3559,10 +3553,10 @@
         <v>22</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3570,10 +3564,10 @@
         <v>23</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3581,10 +3575,10 @@
         <v>24</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3592,10 +3586,10 @@
         <v>25</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3603,21 +3597,21 @@
         <v>26</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -3683,16 +3677,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3700,10 +3694,10 @@
         <v>38</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3711,10 +3705,10 @@
         <v>37</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3722,10 +3716,10 @@
         <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3733,10 +3727,10 @@
         <v>39</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3744,10 +3738,10 @@
         <v>40</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3761,7 +3755,7 @@
         <v>33</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3775,7 +3769,7 @@
         <v>33</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -3846,10 +3840,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>27</v>
@@ -3881,10 +3875,10 @@
         <v>38</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>33</v>
@@ -3910,10 +3904,10 @@
         <v>37</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>33</v>
@@ -3939,22 +3933,22 @@
         <v>35</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="F11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>62</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>33</v>
@@ -3968,13 +3962,13 @@
         <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>33</v>
@@ -3983,7 +3977,7 @@
         <v>33</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>33</v>
@@ -3997,10 +3991,10 @@
         <v>39</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>33</v>
@@ -4026,10 +4020,10 @@
         <v>40</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>33</v>
@@ -4055,10 +4049,10 @@
         <v>31</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>33</v>
@@ -4226,7 +4220,7 @@
     </row>
     <row r="21" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>33</v>
@@ -4468,7 +4462,7 @@
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="12" t="s">
+      <c r="F29" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G29" s="8" t="s">
@@ -4477,7 +4471,7 @@
       <c r="H29" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="I29" s="12" t="s">
+      <c r="I29" s="1" t="s">
         <v>33</v>
       </c>
       <c r="J29" s="1" t="s">
@@ -4489,7 +4483,7 @@
     </row>
     <row r="30" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>33</v>
@@ -4598,10 +4592,10 @@
         <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4620,10 +4614,10 @@
         <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -4631,10 +4625,10 @@
         <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -4653,10 +4647,10 @@
         <v>20</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4664,10 +4658,10 @@
         <v>21</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4675,10 +4669,10 @@
         <v>22</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4686,10 +4680,10 @@
         <v>23</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4697,10 +4691,10 @@
         <v>24</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4708,10 +4702,10 @@
         <v>25</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4719,37 +4713,37 @@
         <v>26</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C23" s="8">
         <v>39619</v>
@@ -4826,16 +4820,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>27</v>
@@ -4861,16 +4855,16 @@
         <v>38</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>33</v>
@@ -4890,16 +4884,16 @@
         <v>37</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>33</v>
@@ -4925,16 +4919,16 @@
         <v>33</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="H11" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>57</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>33</v>
@@ -4948,22 +4942,22 @@
         <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="H12" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>33</v>
@@ -4977,16 +4971,16 @@
         <v>39</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>33</v>
@@ -5006,16 +5000,16 @@
         <v>40</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>33</v>
@@ -5041,13 +5035,13 @@
         <v>33</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>33</v>
@@ -5056,7 +5050,7 @@
         <v>33</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -5127,16 +5121,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>27</v>
@@ -5162,16 +5156,16 @@
         <v>38</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>33</v>
@@ -5191,19 +5185,19 @@
         <v>37</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="H10" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>53</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>33</v>
@@ -5226,10 +5220,10 @@
         <v>33</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>36</v>
@@ -5249,22 +5243,22 @@
         <v>26</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="G12" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>33</v>
@@ -5278,16 +5272,16 @@
         <v>39</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="F13" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>33</v>
@@ -5307,16 +5301,16 @@
         <v>40</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>33</v>
@@ -5342,10 +5336,10 @@
         <v>33</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>33</v>
@@ -5377,10 +5371,10 @@
         <v>33</v>
       </c>
       <c r="F16" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H16" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>53</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1" t="s">
@@ -5400,10 +5394,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5530,50 +5524,24 @@
     </row>
     <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>33</v>
+        <v>45</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates to data release schedules to address inconsistencies and notes from AGAGErs
</commit_message>
<xml_diff>
--- a/data/agage/data_combination.xlsx
+++ b/data/agage/data_combination.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/code/agage-archive/data/agage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2621D0-9261-4C4E-9502-C0C39AF51D5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04FC0CF-0AC3-7343-83F2-8A49BBB7AEAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2060" yWindow="500" windowWidth="36340" windowHeight="19760" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2020" yWindow="500" windowWidth="36340" windowHeight="19760" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CGO" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="137">
   <si>
     <t># File specifying when to use the various ALE/GAGE/AGAGE instruments</t>
   </si>
@@ -241,12 +241,6 @@
   </si>
   <si>
     <t>1984-01-01 00:00</t>
-  </si>
-  <si>
-    <t>1985-11-01 00:00</t>
-  </si>
-  <si>
-    <t>1984-05-10 00:00</t>
   </si>
   <si>
     <t>GCMS-MteCimone start</t>
@@ -876,10 +870,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:Q32"/>
+  <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -954,16 +948,16 @@
         <v>28</v>
       </c>
       <c r="H8" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="J8" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="K8" s="3" t="s">
         <v>133</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>135</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>8</v>
@@ -995,13 +989,13 @@
         <v>33</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H9" s="10" t="s">
         <v>33</v>
@@ -1028,7 +1022,7 @@
         <v>33</v>
       </c>
       <c r="P9" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1036,19 +1030,19 @@
         <v>26</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H10" s="10" t="s">
         <v>33</v>
@@ -1069,7 +1063,7 @@
         <v>33</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>33</v>
@@ -1083,16 +1077,16 @@
         <v>38</v>
       </c>
       <c r="C11" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="E11" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="F11" s="10" t="s">
         <v>121</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>123</v>
       </c>
       <c r="H11" s="10" t="s">
         <v>33</v>
@@ -1130,16 +1124,16 @@
         <v>37</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H12" s="10" t="s">
         <v>33</v>
@@ -1184,10 +1178,10 @@
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>53</v>
@@ -1228,16 +1222,16 @@
         <v>39</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H14" s="10" t="s">
         <v>33</v>
@@ -1275,16 +1269,16 @@
         <v>40</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H15" s="10" t="s">
         <v>33</v>
@@ -1352,10 +1346,10 @@
         <v>33</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="P16" s="1" t="s">
         <v>33</v>
@@ -1399,10 +1393,10 @@
         <v>33</v>
       </c>
       <c r="M17" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="N17" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="P17" s="1" t="s">
         <v>33</v>
@@ -1446,10 +1440,10 @@
         <v>33</v>
       </c>
       <c r="M18" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="N18" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="P18" s="1" t="s">
         <v>33</v>
@@ -1493,10 +1487,10 @@
         <v>33</v>
       </c>
       <c r="M19" s="10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="N19" s="10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="P19" s="1" t="s">
         <v>33</v>
@@ -1540,10 +1534,10 @@
         <v>33</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="P20" s="1" t="s">
         <v>33</v>
@@ -1554,7 +1548,7 @@
     </row>
     <row r="21" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>33</v>
@@ -1588,10 +1582,10 @@
       </c>
       <c r="L21" s="1"/>
       <c r="M21" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="N21" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="P21" s="1" t="s">
         <v>33</v>
@@ -1635,10 +1629,10 @@
         <v>33</v>
       </c>
       <c r="M22" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="N22" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="P22" s="1" t="s">
         <v>33</v>
@@ -1682,10 +1676,10 @@
         <v>33</v>
       </c>
       <c r="M23" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="N23" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="P23" s="1" t="s">
         <v>33</v>
@@ -1729,10 +1723,10 @@
         <v>33</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="P24" s="1" t="s">
         <v>33</v>
@@ -1776,10 +1770,10 @@
         <v>33</v>
       </c>
       <c r="M25" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="N25" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="P25" s="1" t="s">
         <v>33</v>
@@ -1823,10 +1817,10 @@
         <v>33</v>
       </c>
       <c r="M26" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="N26" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="P26" s="1" t="s">
         <v>33</v>
@@ -1870,10 +1864,10 @@
         <v>33</v>
       </c>
       <c r="M27" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="N27" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="P27" s="1" t="s">
         <v>33</v>
@@ -1917,10 +1911,10 @@
         <v>33</v>
       </c>
       <c r="M28" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="N28" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="P28" s="1" t="s">
         <v>33</v>
@@ -1931,7 +1925,7 @@
     </row>
     <row r="29" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>25</v>
+        <v>114</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>33</v>
@@ -1945,8 +1939,12 @@
       <c r="E29" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
+      <c r="F29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="H29" s="10" t="s">
         <v>33</v>
       </c>
@@ -1959,17 +1957,11 @@
       <c r="K29" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="L29" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="M29" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="N29" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="O29" s="1" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="P29" s="1" t="s">
         <v>33</v>
@@ -1978,56 +1970,56 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H30" s="10" t="s">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G30" s="2" t="s">
         <v>33</v>
       </c>
       <c r="I30" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="J30" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="K30" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="M30" s="10" t="s">
-        <v>130</v>
+        <v>135</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="N30" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="P30" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q30" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="P30" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q30" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>44</v>
+        <v>134</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>33</v>
@@ -2041,82 +2033,35 @@
       <c r="E31" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I31" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="L31" s="2" t="s">
+      <c r="G31" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J31" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="K31"/>
+      <c r="L31" t="s">
         <v>33</v>
       </c>
       <c r="M31" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="N31" s="10" t="s">
-        <v>137</v>
+      <c r="N31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O31" t="s">
+        <v>33</v>
       </c>
       <c r="P31" s="2" t="s">
         <v>33</v>
       </c>
       <c r="Q31" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G32" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J32" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="K32"/>
-      <c r="L32" t="s">
-        <v>33</v>
-      </c>
-      <c r="M32" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N32" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="O32" t="s">
-        <v>33</v>
-      </c>
-      <c r="P32" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q32" s="2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2189,16 +2134,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>10</v>
@@ -2210,10 +2155,10 @@
     </row>
     <row r="9" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10" t="s">
@@ -2229,10 +2174,10 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11" t="s">
@@ -2257,10 +2202,10 @@
         <v>33</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
@@ -2269,10 +2214,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11" t="s">
@@ -2288,10 +2233,10 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11" t="s">
@@ -2309,7 +2254,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11" t="s">
@@ -2339,17 +2284,17 @@
         <v>33</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11" t="s">
@@ -2367,7 +2312,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11" t="s">
@@ -2382,10 +2327,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11" t="s">
@@ -2403,7 +2348,7 @@
         <v>64</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C19" s="11"/>
       <c r="D19" s="11" t="s">
@@ -2421,7 +2366,7 @@
         <v>16</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11" t="s">
@@ -2436,10 +2381,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="11" t="s">
@@ -2454,10 +2399,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="11" t="s">
@@ -2472,10 +2417,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11" t="s">
@@ -2493,7 +2438,7 @@
         <v>17</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11" t="s">
@@ -2508,7 +2453,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>33</v>
@@ -2535,7 +2480,7 @@
         <v>19</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="11" t="s">
@@ -2550,10 +2495,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="11" t="s">
@@ -2568,10 +2513,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C28" s="11"/>
       <c r="D28" s="11" t="s">
@@ -2589,7 +2534,7 @@
         <v>20</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C29" s="11"/>
       <c r="D29" s="11" t="s">
@@ -2607,7 +2552,7 @@
         <v>22</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="11" t="s">
@@ -2625,7 +2570,7 @@
         <v>23</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C31" s="11"/>
       <c r="D31" s="11" t="s">
@@ -2640,10 +2585,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="11" t="s">
@@ -2661,7 +2606,7 @@
         <v>24</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C33" s="11"/>
       <c r="D33" s="11" t="s">
@@ -2679,7 +2624,7 @@
         <v>25</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="11" t="s">
@@ -2694,10 +2639,10 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C35" s="11"/>
       <c r="D35" s="11" t="s">
@@ -2712,10 +2657,10 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C36" s="11"/>
       <c r="D36" s="11" t="s">
@@ -2730,10 +2675,10 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C37" s="11"/>
       <c r="D37" s="11" t="s">
@@ -2748,10 +2693,10 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="11" t="s">
@@ -2766,10 +2711,10 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="11" t="s">
@@ -2784,10 +2729,10 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C40" s="11"/>
       <c r="D40" s="11" t="s">
@@ -2802,10 +2747,10 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C41" s="11"/>
       <c r="D41" s="11" t="s">
@@ -2820,10 +2765,10 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C42" s="11"/>
       <c r="D42" s="11" t="s">
@@ -2838,10 +2783,10 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C43" s="11"/>
       <c r="D43" s="11" t="s">
@@ -2860,7 +2805,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B44" s="9" t="s">
         <v>33</v>
@@ -2884,10 +2829,10 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C45" s="11"/>
       <c r="D45" s="11" t="s">
@@ -3142,8 +3087,8 @@
   </sheetPr>
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3264,7 +3209,7 @@
     </row>
     <row r="14" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
@@ -3437,10 +3382,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>10</v>
@@ -3454,10 +3399,10 @@
         <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3465,10 +3410,10 @@
         <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3476,10 +3421,10 @@
         <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3487,10 +3432,10 @@
         <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3498,10 +3443,10 @@
         <v>17</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3509,10 +3454,10 @@
         <v>18</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3520,10 +3465,10 @@
         <v>19</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3531,10 +3476,10 @@
         <v>20</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3542,10 +3487,10 @@
         <v>21</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3553,10 +3498,10 @@
         <v>22</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3564,10 +3509,10 @@
         <v>23</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3575,10 +3520,10 @@
         <v>24</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3586,10 +3531,10 @@
         <v>25</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3597,21 +3542,21 @@
         <v>26</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -3624,9 +3569,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3744,34 +3691,6 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3782,10 +3701,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4220,7 +4139,7 @@
     </row>
     <row r="21" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>33</v>
@@ -4452,7 +4371,7 @@
     </row>
     <row r="29" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>25</v>
+        <v>114</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>33</v>
@@ -4460,53 +4379,22 @@
       <c r="C29" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H29" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>33</v>
+      <c r="D29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G29" s="8">
+        <v>37940.625</v>
+      </c>
+      <c r="H29" s="8">
+        <v>37940.625</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>33</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G30" s="8">
-        <v>37940.625</v>
-      </c>
-      <c r="H30" s="8">
-        <v>37940.625</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K30" s="1" t="s">
         <v>33</v>
       </c>
     </row>
@@ -4721,7 +4609,7 @@
     </row>
     <row r="21" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>62</v>
@@ -5394,10 +5282,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5501,13 +5389,10 @@
     </row>
     <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>33</v>
@@ -5515,33 +5400,13 @@
       <c r="E10" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="F10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="H10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H11" s="1" t="s">
         <v>43</v>
       </c>
     </row>
@@ -5555,10 +5420,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:O16"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5685,91 +5550,6 @@
       </c>
       <c r="O11" s="6"/>
     </row>
-    <row r="12" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" t="s">
-        <v>33</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added ability to interleave different instruments when they are being combined. Demonstrated with CMN
</commit_message>
<xml_diff>
--- a/data/agage/data_combination.xlsx
+++ b/data/agage/data_combination.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/code/agage-archive/data/agage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04FC0CF-0AC3-7343-83F2-8A49BBB7AEAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B35B142-BDAC-1646-B5D0-599D015532AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2020" yWindow="500" windowWidth="36340" windowHeight="19760" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CGO" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="125">
   <si>
     <t># File specifying when to use the various ALE/GAGE/AGAGE instruments</t>
   </si>
@@ -249,48 +249,9 @@
     <t>GCMS-MteCimone end</t>
   </si>
   <si>
-    <t>2023-12-20 00:47</t>
-  </si>
-  <si>
     <t>2022-10-09 08:19</t>
   </si>
   <si>
-    <t>2023-12-20 00:48</t>
-  </si>
-  <si>
-    <t>2023-12-20 00:49</t>
-  </si>
-  <si>
-    <t>2023-12-20 00:50</t>
-  </si>
-  <si>
-    <t>2023-12-20 00:51</t>
-  </si>
-  <si>
-    <t>2023-12-20 00:52</t>
-  </si>
-  <si>
-    <t>2023-12-20 00:53</t>
-  </si>
-  <si>
-    <t>2023-12-20 00:54</t>
-  </si>
-  <si>
-    <t>2023-12-20 00:55</t>
-  </si>
-  <si>
-    <t>2023-12-20 00:56</t>
-  </si>
-  <si>
-    <t>2023-12-20 00:57</t>
-  </si>
-  <si>
-    <t>2023-12-20 00:58</t>
-  </si>
-  <si>
-    <t>2023-12-20 00:59</t>
-  </si>
-  <si>
     <t>2010-06-01 00:00</t>
   </si>
   <si>
@@ -454,6 +415,9 @@
   </si>
   <si>
     <t>2015-04-24 01:30</t>
+  </si>
+  <si>
+    <t>2023-10-04 00:00</t>
   </si>
 </sst>
 </file>
@@ -948,16 +912,16 @@
         <v>28</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>8</v>
@@ -989,13 +953,13 @@
         <v>33</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="H9" s="10" t="s">
         <v>33</v>
@@ -1022,7 +986,7 @@
         <v>33</v>
       </c>
       <c r="P9" s="10" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1030,19 +994,19 @@
         <v>26</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="H10" s="10" t="s">
         <v>33</v>
@@ -1063,7 +1027,7 @@
         <v>33</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>33</v>
@@ -1077,16 +1041,16 @@
         <v>38</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="H11" s="10" t="s">
         <v>33</v>
@@ -1124,16 +1088,16 @@
         <v>37</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="H12" s="10" t="s">
         <v>33</v>
@@ -1178,10 +1142,10 @@
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="10" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>53</v>
@@ -1222,16 +1186,16 @@
         <v>39</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="H14" s="10" t="s">
         <v>33</v>
@@ -1269,16 +1233,16 @@
         <v>40</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="H15" s="10" t="s">
         <v>33</v>
@@ -1346,10 +1310,10 @@
         <v>33</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="P16" s="1" t="s">
         <v>33</v>
@@ -1393,10 +1357,10 @@
         <v>33</v>
       </c>
       <c r="M17" s="10" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="N17" s="10" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="P17" s="1" t="s">
         <v>33</v>
@@ -1440,10 +1404,10 @@
         <v>33</v>
       </c>
       <c r="M18" s="10" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="N18" s="10" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="P18" s="1" t="s">
         <v>33</v>
@@ -1487,10 +1451,10 @@
         <v>33</v>
       </c>
       <c r="M19" s="10" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="N19" s="10" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="P19" s="1" t="s">
         <v>33</v>
@@ -1534,10 +1498,10 @@
         <v>33</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="P20" s="1" t="s">
         <v>33</v>
@@ -1548,7 +1512,7 @@
     </row>
     <row r="21" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>33</v>
@@ -1582,10 +1546,10 @@
       </c>
       <c r="L21" s="1"/>
       <c r="M21" s="10" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="N21" s="10" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="P21" s="1" t="s">
         <v>33</v>
@@ -1629,10 +1593,10 @@
         <v>33</v>
       </c>
       <c r="M22" s="10" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="N22" s="10" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="P22" s="1" t="s">
         <v>33</v>
@@ -1676,10 +1640,10 @@
         <v>33</v>
       </c>
       <c r="M23" s="10" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="N23" s="10" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="P23" s="1" t="s">
         <v>33</v>
@@ -1723,10 +1687,10 @@
         <v>33</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="P24" s="1" t="s">
         <v>33</v>
@@ -1770,10 +1734,10 @@
         <v>33</v>
       </c>
       <c r="M25" s="10" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="N25" s="10" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="P25" s="1" t="s">
         <v>33</v>
@@ -1817,10 +1781,10 @@
         <v>33</v>
       </c>
       <c r="M26" s="10" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="N26" s="10" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="P26" s="1" t="s">
         <v>33</v>
@@ -1864,10 +1828,10 @@
         <v>33</v>
       </c>
       <c r="M27" s="10" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="N27" s="10" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="P27" s="1" t="s">
         <v>33</v>
@@ -1911,10 +1875,10 @@
         <v>33</v>
       </c>
       <c r="M28" s="10" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="N28" s="10" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="P28" s="1" t="s">
         <v>33</v>
@@ -1925,7 +1889,7 @@
     </row>
     <row r="29" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>33</v>
@@ -1958,10 +1922,10 @@
         <v>33</v>
       </c>
       <c r="M29" s="10" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="N29" s="10" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="P29" s="1" t="s">
         <v>33</v>
@@ -1993,7 +1957,7 @@
         <v>33</v>
       </c>
       <c r="I30" s="10" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="J30" s="2" t="s">
         <v>33</v>
@@ -2008,7 +1972,7 @@
         <v>33</v>
       </c>
       <c r="N30" s="10" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="P30" s="2" t="s">
         <v>33</v>
@@ -2019,7 +1983,7 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>33</v>
@@ -2034,7 +1998,7 @@
         <v>33</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>33</v>
@@ -2043,7 +2007,7 @@
         <v>33</v>
       </c>
       <c r="J31" s="10" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="K31"/>
       <c r="L31" t="s">
@@ -2134,16 +2098,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>10</v>
@@ -2155,10 +2119,10 @@
     </row>
     <row r="9" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10" t="s">
@@ -2174,10 +2138,10 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11" t="s">
@@ -2202,10 +2166,10 @@
         <v>33</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
@@ -2214,10 +2178,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11" t="s">
@@ -2233,10 +2197,10 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11" t="s">
@@ -2254,7 +2218,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11" t="s">
@@ -2284,17 +2248,17 @@
         <v>33</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11" t="s">
@@ -2312,7 +2276,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11" t="s">
@@ -2327,10 +2291,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11" t="s">
@@ -2348,7 +2312,7 @@
         <v>64</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="C19" s="11"/>
       <c r="D19" s="11" t="s">
@@ -2366,7 +2330,7 @@
         <v>16</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11" t="s">
@@ -2381,10 +2345,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="11" t="s">
@@ -2399,10 +2363,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="11" t="s">
@@ -2417,10 +2381,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11" t="s">
@@ -2438,7 +2402,7 @@
         <v>17</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11" t="s">
@@ -2453,7 +2417,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>33</v>
@@ -2480,7 +2444,7 @@
         <v>19</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="11" t="s">
@@ -2495,10 +2459,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="11" t="s">
@@ -2513,10 +2477,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="C28" s="11"/>
       <c r="D28" s="11" t="s">
@@ -2534,7 +2498,7 @@
         <v>20</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="C29" s="11"/>
       <c r="D29" s="11" t="s">
@@ -2552,7 +2516,7 @@
         <v>22</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="11" t="s">
@@ -2570,7 +2534,7 @@
         <v>23</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C31" s="11"/>
       <c r="D31" s="11" t="s">
@@ -2585,10 +2549,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="11" t="s">
@@ -2606,7 +2570,7 @@
         <v>24</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C33" s="11"/>
       <c r="D33" s="11" t="s">
@@ -2624,7 +2588,7 @@
         <v>25</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="11" t="s">
@@ -2639,10 +2603,10 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C35" s="11"/>
       <c r="D35" s="11" t="s">
@@ -2657,10 +2621,10 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C36" s="11"/>
       <c r="D36" s="11" t="s">
@@ -2675,10 +2639,10 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C37" s="11"/>
       <c r="D37" s="11" t="s">
@@ -2693,10 +2657,10 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="11" t="s">
@@ -2711,10 +2675,10 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="11" t="s">
@@ -2729,10 +2693,10 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C40" s="11"/>
       <c r="D40" s="11" t="s">
@@ -2747,10 +2711,10 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C41" s="11"/>
       <c r="D41" s="11" t="s">
@@ -2765,10 +2729,10 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C42" s="11"/>
       <c r="D42" s="11" t="s">
@@ -2783,10 +2747,10 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C43" s="11"/>
       <c r="D43" s="11" t="s">
@@ -2805,7 +2769,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="B44" s="9" t="s">
         <v>33</v>
@@ -2829,10 +2793,10 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C45" s="11"/>
       <c r="D45" s="11" t="s">
@@ -3087,7 +3051,7 @@
   </sheetPr>
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -3209,7 +3173,7 @@
     </row>
     <row r="14" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
@@ -3329,8 +3293,8 @@
   </sheetPr>
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3398,166 +3362,196 @@
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="9"/>
+      <c r="C9" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="E9" s="9"/>
     </row>
     <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="9"/>
     </row>
     <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="9"/>
     </row>
     <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" s="9"/>
     </row>
     <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="9"/>
     </row>
     <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="B14" s="9"/>
+      <c r="C14" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="9"/>
     </row>
     <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="9"/>
     </row>
     <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="9"/>
+      <c r="C16" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="9"/>
+    </row>
+    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="9"/>
+      <c r="C17" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="9"/>
+      <c r="C18" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="9"/>
+    </row>
+    <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="9"/>
+      <c r="C19" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="9"/>
+    </row>
+    <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="9"/>
+      <c r="C20" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="9"/>
+    </row>
+    <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="9"/>
+      <c r="C21" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="9"/>
+    </row>
+    <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="9"/>
+      <c r="C22" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" s="9"/>
+    </row>
+    <row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>69</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="B23" s="9"/>
+      <c r="C23" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4139,7 +4133,7 @@
     </row>
     <row r="21" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>33</v>
@@ -4371,7 +4365,7 @@
     </row>
     <row r="29" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>33</v>
@@ -4609,7 +4603,7 @@
     </row>
     <row r="21" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>62</v>

</xml_diff>

<commit_message>
Added Picarros 1-3 in release schedule and data_combination
</commit_message>
<xml_diff>
--- a/data/agage/data_combination.xlsx
+++ b/data/agage/data_combination.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/code/agage-archive/data/agage/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B35B142-BDAC-1646-B5D0-599D015532AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66CAEFE-DEFA-EF4C-8BE4-0E82B265C742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="580" yWindow="500" windowWidth="31900" windowHeight="19760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CGO" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1191" uniqueCount="130">
   <si>
     <t># File specifying when to use the various ALE/GAGE/AGAGE instruments</t>
   </si>
@@ -417,7 +417,22 @@
     <t>2015-04-24 01:30</t>
   </si>
   <si>
+    <t>Picarro-1 start</t>
+  </si>
+  <si>
+    <t>Picarro-1 end</t>
+  </si>
+  <si>
     <t>2023-10-04 00:00</t>
+  </si>
+  <si>
+    <t>Picarro-2 start</t>
+  </si>
+  <si>
+    <t>Picarro-2 end</t>
+  </si>
+  <si>
+    <t>2024-01-01 00:00</t>
   </si>
 </sst>
 </file>
@@ -834,10 +849,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:Q31"/>
+  <dimension ref="A1:S31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -851,45 +866,46 @@
     <col min="14" max="14" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -936,13 +952,19 @@
         <v>11</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>29</v>
+        <v>124</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
@@ -988,8 +1010,12 @@
       <c r="P9" s="10" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R9" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="S9" s="2"/>
+    </row>
+    <row r="10" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -1035,8 +1061,14 @@
       <c r="Q10" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>38</v>
       </c>
@@ -1082,8 +1114,14 @@
       <c r="Q11" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>37</v>
       </c>
@@ -1129,8 +1167,14 @@
       <c r="Q12" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
@@ -1180,8 +1224,14 @@
       <c r="Q13" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>39</v>
       </c>
@@ -1227,8 +1277,14 @@
       <c r="Q14" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>40</v>
       </c>
@@ -1274,8 +1330,14 @@
       <c r="Q15" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -1321,8 +1383,14 @@
       <c r="Q16" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -1368,8 +1436,14 @@
       <c r="Q17" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -1415,8 +1489,14 @@
       <c r="Q18" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -1462,8 +1542,14 @@
       <c r="Q19" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -1509,8 +1595,14 @@
       <c r="Q20" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>71</v>
       </c>
@@ -1557,8 +1649,14 @@
       <c r="Q21" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
@@ -1604,8 +1702,14 @@
       <c r="Q22" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
@@ -1651,8 +1755,14 @@
       <c r="Q23" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S23" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
@@ -1698,8 +1808,14 @@
       <c r="Q24" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S24" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
@@ -1745,8 +1861,14 @@
       <c r="Q25" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S25" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>22</v>
       </c>
@@ -1792,8 +1914,14 @@
       <c r="Q26" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S26" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>23</v>
       </c>
@@ -1839,8 +1967,14 @@
       <c r="Q27" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S27" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>24</v>
       </c>
@@ -1886,8 +2020,14 @@
       <c r="Q28" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S28" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>101</v>
       </c>
@@ -1933,8 +2073,14 @@
       <c r="Q29" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S29" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>44</v>
       </c>
@@ -1980,8 +2126,14 @@
       <c r="Q30" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R30" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="S30" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>121</v>
       </c>
@@ -2026,6 +2178,12 @@
         <v>33</v>
       </c>
       <c r="Q31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="S31" s="2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3293,8 +3451,8 @@
   </sheetPr>
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3362,196 +3520,166 @@
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="9"/>
       <c r="C9" s="10" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E9" s="9"/>
     </row>
     <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="9"/>
       <c r="C10" s="10" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="9"/>
     </row>
     <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="9"/>
       <c r="C11" s="10" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E11" s="9"/>
     </row>
     <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="9"/>
       <c r="C12" s="10" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E12" s="9"/>
     </row>
     <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="9"/>
       <c r="C13" s="10" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E13" s="9"/>
     </row>
     <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="9"/>
       <c r="C14" s="10" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E14" s="9"/>
     </row>
     <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="9"/>
       <c r="C15" s="10" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E15" s="9"/>
     </row>
     <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="9"/>
       <c r="C16" s="10" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E16" s="9"/>
-    </row>
-    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="9"/>
       <c r="C17" s="10" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="9"/>
-    </row>
-    <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="9"/>
       <c r="C18" s="10" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E18" s="9"/>
-    </row>
-    <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="9"/>
       <c r="C19" s="10" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="9"/>
-    </row>
-    <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="9"/>
       <c r="C20" s="10" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E20" s="9"/>
-    </row>
-    <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="9"/>
       <c r="C21" s="10" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E21" s="9"/>
-    </row>
-    <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="9"/>
       <c r="C22" s="10" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E22" s="9"/>
-    </row>
-    <row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B23" s="9"/>
       <c r="C23" s="10" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E23" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added release schedule for TAC MD CO and SF6, and added preprocessing to copy over the relevant MD files for TAC and TOB on DAGAGE2 (Issue #88)
</commit_message>
<xml_diff>
--- a/data/agage/data_combination.xlsx
+++ b/data/agage/data_combination.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="CGO"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="112">
   <si>
     <t># File specifying when to use the various ALE/GAGE/AGAGE instruments</t>
   </si>
@@ -203,6 +203,9 @@
     <t>2016-09-02 21:00</t>
   </si>
   <si>
+    <t>2018-03-14 00:00</t>
+  </si>
+  <si>
     <t>co</t>
   </si>
   <si>
@@ -252,9 +255,6 @@
   </si>
   <si>
     <t>2010-11-01 00:00</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>2017-02-15 00:00</t>
@@ -367,7 +367,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -378,6 +378,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -447,13 +453,13 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -462,7 +468,7 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -474,19 +480,19 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="22" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="22" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="22" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="22" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -495,7 +501,7 @@
     <xf xfId="0" numFmtId="22" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="22" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="22" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -993,16 +999,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>46</v>
@@ -1157,7 +1163,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="1" t="s">
@@ -1212,7 +1218,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="1" t="s">
@@ -1283,7 +1289,7 @@
         <v>99</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>33</v>
@@ -1304,7 +1310,7 @@
         <v>33</v>
       </c>
       <c r="N13" s="12" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>33</v>
@@ -1324,7 +1330,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="1" t="s">
@@ -3758,21 +3764,21 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
       <c r="A9" s="13" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="4" t="s">
@@ -3785,7 +3791,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
       <c r="A10" s="13" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="4" t="s">
@@ -3811,7 +3817,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
       <c r="A12" s="13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="4" t="s">
@@ -3974,10 +3980,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>46</v>
@@ -4006,7 +4012,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
       <c r="A9" s="13" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="1" t="s">
@@ -4037,7 +4043,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
       <c r="A10" s="13" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="1" t="s">
@@ -4109,7 +4115,7 @@
         <v>80</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>33</v>
@@ -4118,7 +4124,7 @@
         <v>33</v>
       </c>
       <c r="H12" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="1" t="s">
@@ -4130,7 +4136,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
       <c r="A13" s="13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="1" t="s">
@@ -4965,7 +4971,7 @@
   </sheetPr>
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5092,16 +5098,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>46</v>
@@ -5124,20 +5130,20 @@
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="13" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="1" t="s">
@@ -5155,20 +5161,20 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="13" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="1" t="s">
@@ -5196,16 +5202,16 @@
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="1" t="s">
@@ -5221,22 +5227,22 @@
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="1" t="s">
@@ -5248,20 +5254,20 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="1" t="s">
@@ -5283,16 +5289,16 @@
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="1" t="s">
@@ -5324,9 +5330,7 @@
       <c r="E15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F15" s="14" t="s">
-        <v>76</v>
-      </c>
+      <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
         <v>77</v>
       </c>
@@ -5480,16 +5484,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>46</v>
@@ -5512,20 +5516,20 @@
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
       <c r="A9" s="13" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="4" t="s">
@@ -5543,24 +5547,24 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
       <c r="A10" s="13" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>33</v>
@@ -5584,10 +5588,10 @@
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G11" s="12" t="s">
         <v>54</v>
@@ -5609,22 +5613,22 @@
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="1" t="s">
@@ -5636,20 +5640,20 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
       <c r="A13" s="13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="4" t="s">
@@ -5671,16 +5675,16 @@
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="1" t="s">
@@ -5708,10 +5712,10 @@
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="1" t="s">
@@ -5744,11 +5748,11 @@
         <v>33</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1" t="s">
@@ -5768,16 +5772,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="6" width="11.147857142857141" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="7" width="15.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="15.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="17.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="24.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="26.433571428571426" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="6" width="17.005" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="6" width="15.576428571428572" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="6" width="11.147857142857141" customWidth="1" bestFit="1"/>
@@ -5930,30 +5934,55 @@
       </c>
       <c r="I9" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="1" t="s">
-        <v>59</v>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+      <c r="A10" s="14" t="s">
+        <v>35</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="A11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" s="1" t="s">
+      <c r="D11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="I10" s="2"/>
+      <c r="I11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5988,7 +6017,7 @@
     <col min="15" max="15" style="11" width="12.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6007,7 +6036,7 @@
       <c r="N1" s="2"/>
       <c r="O1" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -6026,7 +6055,7 @@
       <c r="N2" s="2"/>
       <c r="O2" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -6045,7 +6074,7 @@
       <c r="N3" s="2"/>
       <c r="O3" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -6064,7 +6093,7 @@
       <c r="N4" s="2"/>
       <c r="O4" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -6083,7 +6112,7 @@
       <c r="N5" s="2"/>
       <c r="O5" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -6102,7 +6131,7 @@
       <c r="N6" s="2"/>
       <c r="O6" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
combination: reformat dates to text
</commit_message>
<xml_diff>
--- a/data/agage/data_combination.xlsx
+++ b/data/agage/data_combination.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JOEPIT~1\AppData\Local\Temp\scp22246\user\home\zh21490\agage-archive\data\agage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6AD726-5333-41D2-9C6F-BAFFAFB80A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AADC5FAB-45E5-4C2D-AB45-915942457C75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CGO" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1181" uniqueCount="119">
   <si>
     <t># File specifying when to use the various ALE/GAGE/AGAGE instruments</t>
   </si>
@@ -372,6 +372,21 @@
   </si>
   <si>
     <t>cfc-114</t>
+  </si>
+  <si>
+    <t>2008-05-09 17:30</t>
+  </si>
+  <si>
+    <t>2008-08-15 00:00</t>
+  </si>
+  <si>
+    <t>2008-06-20 00:00</t>
+  </si>
+  <si>
+    <t>2003-11-15 03:00</t>
+  </si>
+  <si>
+    <t>2005-01-12 00:00</t>
   </si>
 </sst>
 </file>
@@ -456,7 +471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -504,6 +519,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="22" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -813,8 +831,8 @@
   </sheetPr>
   <dimension ref="A1:S31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3263,7 +3281,7 @@
   </sheetPr>
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -3803,7 +3821,9 @@
   </sheetPr>
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4174,11 +4194,11 @@
       <c r="E16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="14">
-        <v>37940.125</v>
-      </c>
-      <c r="H16" s="14">
-        <v>37940.125</v>
+      <c r="G16" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="H16" s="17" t="s">
+        <v>117</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>33</v>
@@ -4203,11 +4223,11 @@
       <c r="E17" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="14">
-        <v>37940.125</v>
-      </c>
-      <c r="H17" s="14">
-        <v>37940.125</v>
+      <c r="G17" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>117</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>33</v>
@@ -4232,11 +4252,11 @@
       <c r="E18" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="14">
-        <v>37940.125</v>
-      </c>
-      <c r="H18" s="14">
-        <v>37940.125</v>
+      <c r="G18" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="H18" s="17" t="s">
+        <v>117</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>33</v>
@@ -4261,11 +4281,11 @@
       <c r="E19" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G19" s="14">
-        <v>38364</v>
-      </c>
-      <c r="H19" s="14">
-        <v>38364</v>
+      <c r="G19" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="H19" s="17" t="s">
+        <v>118</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>33</v>
@@ -4290,11 +4310,11 @@
       <c r="E20" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="14">
-        <v>37940.125</v>
-      </c>
-      <c r="H20" s="14">
-        <v>37940.125</v>
+      <c r="G20" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>117</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>33</v>
@@ -4319,11 +4339,11 @@
       <c r="E21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G21" s="14">
-        <v>37940.125</v>
-      </c>
-      <c r="H21" s="14">
-        <v>37940.125</v>
+      <c r="G21" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>117</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>33</v>
@@ -4348,11 +4368,11 @@
       <c r="E22" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G22" s="14">
-        <v>37940.125</v>
-      </c>
-      <c r="H22" s="14">
-        <v>37940.125</v>
+      <c r="G22" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="H22" s="17" t="s">
+        <v>117</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>33</v>
@@ -4377,11 +4397,11 @@
       <c r="E23" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G23" s="14">
-        <v>37940.125</v>
-      </c>
-      <c r="H23" s="14">
-        <v>37940.125</v>
+      <c r="G23" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>117</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>33</v>
@@ -4406,11 +4426,11 @@
       <c r="E24" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G24" s="14">
-        <v>37940.125</v>
-      </c>
-      <c r="H24" s="14">
-        <v>37940.125</v>
+      <c r="G24" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>117</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>33</v>
@@ -4435,11 +4455,11 @@
       <c r="E25" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G25" s="14">
-        <v>37940.125</v>
-      </c>
-      <c r="H25" s="14">
-        <v>37940.125</v>
+      <c r="G25" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="H25" s="17" t="s">
+        <v>117</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>33</v>
@@ -4464,11 +4484,11 @@
       <c r="E26" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G26" s="14">
-        <v>37940.125</v>
-      </c>
-      <c r="H26" s="14">
-        <v>37940.125</v>
+      <c r="G26" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="H26" s="17" t="s">
+        <v>117</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>33</v>
@@ -4493,11 +4513,11 @@
       <c r="E27" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G27" s="14">
-        <v>37940.125</v>
-      </c>
-      <c r="H27" s="14">
-        <v>37940.125</v>
+      <c r="G27" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="H27" s="17" t="s">
+        <v>117</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>33</v>
@@ -4522,11 +4542,11 @@
       <c r="E28" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G28" s="14">
-        <v>37940.125</v>
-      </c>
-      <c r="H28" s="14">
-        <v>37940.125</v>
+      <c r="G28" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="H28" s="17" t="s">
+        <v>117</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>33</v>
@@ -4551,11 +4571,11 @@
       <c r="E29" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G29" s="14">
-        <v>37940.125</v>
-      </c>
-      <c r="H29" s="14">
-        <v>37940.125</v>
+      <c r="G29" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="H29" s="17" t="s">
+        <v>117</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>33</v>
@@ -4576,7 +4596,9 @@
   </sheetPr>
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4657,10 +4679,10 @@
       <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="17" t="s">
         <v>78</v>
       </c>
     </row>
@@ -4668,21 +4690,21 @@
       <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="14">
-        <v>39577.729166666664</v>
-      </c>
-      <c r="D10" s="14">
-        <v>39577.729166666664</v>
+      <c r="C10" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="17" t="s">
         <v>78</v>
       </c>
     </row>
@@ -4690,10 +4712,10 @@
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="17" t="s">
         <v>78</v>
       </c>
     </row>
@@ -4701,21 +4723,21 @@
       <c r="A13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="14">
-        <v>39675</v>
-      </c>
-      <c r="D13" s="14">
-        <v>39675</v>
+      <c r="C13" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="17" t="s">
         <v>78</v>
       </c>
     </row>
@@ -4723,10 +4745,10 @@
       <c r="A15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="17" t="s">
         <v>78</v>
       </c>
     </row>
@@ -4734,10 +4756,10 @@
       <c r="A16" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="17" t="s">
         <v>78</v>
       </c>
     </row>
@@ -4745,10 +4767,10 @@
       <c r="A17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="17" t="s">
         <v>78</v>
       </c>
     </row>
@@ -4756,10 +4778,10 @@
       <c r="A18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="17" t="s">
         <v>78</v>
       </c>
     </row>
@@ -4767,10 +4789,10 @@
       <c r="A19" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="17" t="s">
         <v>78</v>
       </c>
     </row>
@@ -4778,10 +4800,10 @@
       <c r="A20" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="17" t="s">
         <v>78</v>
       </c>
     </row>
@@ -4789,10 +4811,10 @@
       <c r="A21" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="17" t="s">
         <v>78</v>
       </c>
     </row>
@@ -4800,10 +4822,10 @@
       <c r="A22" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="17" t="s">
         <v>78</v>
       </c>
     </row>
@@ -4811,11 +4833,11 @@
       <c r="A23" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="14">
-        <v>39619</v>
-      </c>
-      <c r="D23" s="14">
-        <v>39619</v>
+      <c r="C23" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>